<commit_message>
* add demo server constant * update demo test file
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="number format" sheetId="9" r:id="rId1"/>
@@ -2397,11 +2397,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2070972944"/>
-        <c:axId val="-2070970912"/>
+        <c:axId val="-2099154000"/>
+        <c:axId val="-2126315120"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2070972944"/>
+        <c:axId val="-2099154000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2444,7 +2444,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070970912"/>
+        <c:crossAx val="-2126315120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2452,7 +2452,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070970912"/>
+        <c:axId val="-2126315120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2503,7 +2503,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070972944"/>
+        <c:crossAx val="-2099154000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2844,11 +2844,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124295280"/>
-        <c:axId val="-2123787200"/>
+        <c:axId val="-2099143216"/>
+        <c:axId val="-2099139920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124295280"/>
+        <c:axId val="-2099143216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2891,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123787200"/>
+        <c:crossAx val="-2099139920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2899,7 +2899,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2123787200"/>
+        <c:axId val="-2099139920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,7 +2950,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124295280"/>
+        <c:crossAx val="-2099143216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3291,11 +3291,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2019897488"/>
-        <c:axId val="-2019717680"/>
+        <c:axId val="2028373024"/>
+        <c:axId val="-2124119536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019897488"/>
+        <c:axId val="2028373024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3338,7 +3338,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019717680"/>
+        <c:crossAx val="-2124119536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3346,7 +3346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2019717680"/>
+        <c:axId val="-2124119536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3397,7 +3397,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019897488"/>
+        <c:crossAx val="2028373024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3794,11 +3794,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="-2072976080"/>
-        <c:axId val="2125591168"/>
+        <c:axId val="-2099576048"/>
+        <c:axId val="-2099572800"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="-2072976080"/>
+        <c:axId val="-2099576048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3841,12 +3841,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2125591168"/>
+        <c:crossAx val="-2099572800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2125591168"/>
+        <c:axId val="-2099572800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3897,7 +3897,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072976080"/>
+        <c:crossAx val="-2099576048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4710,11 +4710,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2020051664"/>
-        <c:axId val="-2020048368"/>
+        <c:axId val="-2111732720"/>
+        <c:axId val="-2126362800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2020051664"/>
+        <c:axId val="-2111732720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4757,7 +4757,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020048368"/>
+        <c:crossAx val="-2126362800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4765,7 +4765,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2020048368"/>
+        <c:axId val="-2126362800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4816,7 +4816,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020051664"/>
+        <c:crossAx val="-2111732720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5161,11 +5161,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2020240880"/>
-        <c:axId val="-2080170864"/>
+        <c:axId val="-2122637440"/>
+        <c:axId val="-2122880288"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2020240880"/>
+        <c:axId val="-2122637440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5222,7 +5222,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080170864"/>
+        <c:crossAx val="-2122880288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5230,7 +5230,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080170864"/>
+        <c:axId val="-2122880288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5281,7 +5281,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020240880"/>
+        <c:crossAx val="-2122637440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5659,11 +5659,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2020089504"/>
-        <c:axId val="-2020086448"/>
+        <c:axId val="-2099558624"/>
+        <c:axId val="-2099555344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2020089504"/>
+        <c:axId val="-2099558624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5720,12 +5720,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020086448"/>
+        <c:crossAx val="-2099555344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2020086448"/>
+        <c:axId val="-2099555344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5776,7 +5776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2020089504"/>
+        <c:crossAx val="-2099558624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6172,12 +6172,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2080209776"/>
-        <c:axId val="-2080214000"/>
+        <c:axId val="2028348528"/>
+        <c:axId val="-2122764352"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2080209776"/>
+        <c:axId val="2028348528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6220,7 +6220,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080214000"/>
+        <c:crossAx val="-2122764352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6228,7 +6228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080214000"/>
+        <c:axId val="-2122764352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6279,7 +6279,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080209776"/>
+        <c:crossAx val="2028348528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11705,11 +11705,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table15" displayName="Table15" ref="A2:E6" totalsRowCount="1">
   <autoFilter ref="A2:E5"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11719,11 +11719,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1764" displayName="Table1764" ref="A31:E35" totalsRowCount="1">
   <autoFilter ref="A31:E34"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11733,11 +11733,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1865" displayName="Table1865" ref="G31:K35" totalsRowCount="1">
   <autoFilter ref="G31:K34"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11747,11 +11747,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1966" displayName="Table1966" ref="A38:E42" totalsRowCount="1">
   <autoFilter ref="A38:E41"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11761,11 +11761,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table11167" displayName="Table11167" ref="M24:Q28" totalsRowCount="1">
   <autoFilter ref="M24:Q27"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11775,11 +11775,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table11268" displayName="Table11268" ref="M31:Q35" totalsRowCount="1">
   <autoFilter ref="M31:Q34"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11789,11 +11789,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table16" displayName="Table16" ref="G2:K6" totalsRowCount="1">
   <autoFilter ref="G2:K5"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11803,11 +11803,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table17" displayName="Table17" ref="A9:E13" totalsRowCount="1">
   <autoFilter ref="A9:E12"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11817,11 +11817,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table18" displayName="Table18" ref="G9:K13" totalsRowCount="1">
   <autoFilter ref="G9:K12"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11831,11 +11831,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table19" displayName="Table19" ref="A16:E20" totalsRowCount="1">
   <autoFilter ref="A16:E19"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11845,11 +11845,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table111" displayName="Table111" ref="M2:Q6" totalsRowCount="1">
   <autoFilter ref="M2:Q5"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11859,11 +11859,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table112" displayName="Table112" ref="M9:Q13" totalsRowCount="1">
   <autoFilter ref="M9:Q12"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11873,11 +11873,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1562" displayName="Table1562" ref="A24:E28" totalsRowCount="1">
   <autoFilter ref="A24:E27"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -11887,11 +11887,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1663" displayName="Table1663" ref="G24:K28" totalsRowCount="1">
   <autoFilter ref="G24:K27"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count"/>
+    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -12186,7 +12186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -12438,7 +12438,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15529,16 +15531,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="E60:G67">
-    <cfRule type="colorScale" priority="154">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
     <cfRule type="expression" dxfId="73" priority="155">
       <formula>"&gt;2000"</formula>
     </cfRule>
@@ -16718,10 +16710,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17037,6 +17029,2118 @@
         <v>91000</v>
       </c>
     </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B16" s="96">
+        <v>13</v>
+      </c>
+      <c r="C16" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D16" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E16" s="98">
+        <f>C16-D16</f>
+        <v>26900</v>
+      </c>
+      <c r="F16" s="99">
+        <f>E16</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B17" s="96">
+        <v>19</v>
+      </c>
+      <c r="C17" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D17" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E17" s="98">
+        <f t="shared" ref="E17:E18" si="1">C17-D17</f>
+        <v>40200</v>
+      </c>
+      <c r="F17" s="99">
+        <f>E16+E17</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B18" s="96">
+        <v>25</v>
+      </c>
+      <c r="C18" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D18" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E18" s="98">
+        <f t="shared" si="1"/>
+        <v>91400</v>
+      </c>
+      <c r="F18" s="99">
+        <f>E16+E17+E18</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B19" s="96">
+        <v>22</v>
+      </c>
+      <c r="C19" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D19" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E19" s="98">
+        <f>C19-D19</f>
+        <v>36300</v>
+      </c>
+      <c r="F19" s="100">
+        <f>E19</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B20" s="96">
+        <v>28</v>
+      </c>
+      <c r="C20" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D20" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E20" s="98">
+        <f t="shared" ref="E20:E27" si="2">C20-D20</f>
+        <v>39700</v>
+      </c>
+      <c r="F20" s="100">
+        <f>E19+E20</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B21" s="96">
+        <v>35</v>
+      </c>
+      <c r="C21" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D21" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E21" s="98">
+        <f t="shared" si="2"/>
+        <v>46200</v>
+      </c>
+      <c r="F21" s="100">
+        <f>E19+E20+E21</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B22" s="96">
+        <v>20</v>
+      </c>
+      <c r="C22" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D22" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E22" s="98">
+        <f t="shared" si="2"/>
+        <v>33400</v>
+      </c>
+      <c r="F22" s="101">
+        <f>E22</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B23" s="96">
+        <v>31</v>
+      </c>
+      <c r="C23" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D23" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E23" s="98">
+        <f t="shared" si="2"/>
+        <v>39600</v>
+      </c>
+      <c r="F23" s="101">
+        <f>E22+E23</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B24" s="96">
+        <v>27</v>
+      </c>
+      <c r="C24" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D24" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E24" s="98">
+        <f t="shared" si="2"/>
+        <v>41200</v>
+      </c>
+      <c r="F24" s="101">
+        <f>E22+E23+E24</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B25" s="96">
+        <v>24</v>
+      </c>
+      <c r="C25" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D25" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E25" s="98">
+        <f t="shared" si="2"/>
+        <v>27400</v>
+      </c>
+      <c r="F25" s="102">
+        <f>E25</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B26" s="96">
+        <v>19</v>
+      </c>
+      <c r="C26" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D26" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E26" s="98">
+        <f t="shared" si="2"/>
+        <v>35200</v>
+      </c>
+      <c r="F26" s="102">
+        <f>E25+E26</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B27" s="96">
+        <v>17</v>
+      </c>
+      <c r="C27" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D27" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E27" s="98">
+        <f t="shared" si="2"/>
+        <v>28400</v>
+      </c>
+      <c r="F27" s="102">
+        <f>E25+E26+E27</f>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B28" s="96">
+        <v>13</v>
+      </c>
+      <c r="C28" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D28" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E28" s="98">
+        <f>C28-D28</f>
+        <v>26900</v>
+      </c>
+      <c r="F28" s="99">
+        <f>E28</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B29" s="96">
+        <v>19</v>
+      </c>
+      <c r="C29" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D29" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E29" s="98">
+        <f t="shared" ref="E29:E30" si="3">C29-D29</f>
+        <v>40200</v>
+      </c>
+      <c r="F29" s="99">
+        <f>E28+E29</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B30" s="96">
+        <v>25</v>
+      </c>
+      <c r="C30" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D30" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E30" s="98">
+        <f t="shared" si="3"/>
+        <v>91400</v>
+      </c>
+      <c r="F30" s="99">
+        <f>E28+E29+E30</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B31" s="96">
+        <v>22</v>
+      </c>
+      <c r="C31" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D31" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E31" s="98">
+        <f>C31-D31</f>
+        <v>36300</v>
+      </c>
+      <c r="F31" s="100">
+        <f>E31</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B32" s="96">
+        <v>28</v>
+      </c>
+      <c r="C32" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D32" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E32" s="98">
+        <f t="shared" ref="E32:E39" si="4">C32-D32</f>
+        <v>39700</v>
+      </c>
+      <c r="F32" s="100">
+        <f>E31+E32</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B33" s="96">
+        <v>35</v>
+      </c>
+      <c r="C33" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D33" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E33" s="98">
+        <f t="shared" si="4"/>
+        <v>46200</v>
+      </c>
+      <c r="F33" s="100">
+        <f>E31+E32+E33</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B34" s="96">
+        <v>20</v>
+      </c>
+      <c r="C34" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D34" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E34" s="98">
+        <f t="shared" si="4"/>
+        <v>33400</v>
+      </c>
+      <c r="F34" s="101">
+        <f>E34</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B35" s="96">
+        <v>31</v>
+      </c>
+      <c r="C35" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D35" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E35" s="98">
+        <f t="shared" si="4"/>
+        <v>39600</v>
+      </c>
+      <c r="F35" s="101">
+        <f>E34+E35</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B36" s="96">
+        <v>27</v>
+      </c>
+      <c r="C36" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D36" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E36" s="98">
+        <f t="shared" si="4"/>
+        <v>41200</v>
+      </c>
+      <c r="F36" s="101">
+        <f>E34+E35+E36</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B37" s="96">
+        <v>24</v>
+      </c>
+      <c r="C37" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D37" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E37" s="98">
+        <f t="shared" si="4"/>
+        <v>27400</v>
+      </c>
+      <c r="F37" s="102">
+        <f>E37</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B38" s="96">
+        <v>19</v>
+      </c>
+      <c r="C38" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D38" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E38" s="98">
+        <f t="shared" si="4"/>
+        <v>35200</v>
+      </c>
+      <c r="F38" s="102">
+        <f>E37+E38</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B39" s="96">
+        <v>17</v>
+      </c>
+      <c r="C39" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D39" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E39" s="98">
+        <f t="shared" si="4"/>
+        <v>28400</v>
+      </c>
+      <c r="F39" s="102">
+        <f>E37+E38+E39</f>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B40" s="96">
+        <v>13</v>
+      </c>
+      <c r="C40" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D40" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E40" s="98">
+        <f>C40-D40</f>
+        <v>26900</v>
+      </c>
+      <c r="F40" s="99">
+        <f>E40</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B41" s="96">
+        <v>19</v>
+      </c>
+      <c r="C41" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D41" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E41" s="98">
+        <f t="shared" ref="E41:E42" si="5">C41-D41</f>
+        <v>40200</v>
+      </c>
+      <c r="F41" s="99">
+        <f>E40+E41</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B42" s="96">
+        <v>25</v>
+      </c>
+      <c r="C42" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D42" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E42" s="98">
+        <f t="shared" si="5"/>
+        <v>91400</v>
+      </c>
+      <c r="F42" s="99">
+        <f>E40+E41+E42</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B43" s="96">
+        <v>22</v>
+      </c>
+      <c r="C43" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D43" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E43" s="98">
+        <f>C43-D43</f>
+        <v>36300</v>
+      </c>
+      <c r="F43" s="100">
+        <f>E43</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B44" s="96">
+        <v>28</v>
+      </c>
+      <c r="C44" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D44" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E44" s="98">
+        <f t="shared" ref="E44:E51" si="6">C44-D44</f>
+        <v>39700</v>
+      </c>
+      <c r="F44" s="100">
+        <f>E43+E44</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B45" s="96">
+        <v>35</v>
+      </c>
+      <c r="C45" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D45" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E45" s="98">
+        <f t="shared" si="6"/>
+        <v>46200</v>
+      </c>
+      <c r="F45" s="100">
+        <f>E43+E44+E45</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B46" s="96">
+        <v>20</v>
+      </c>
+      <c r="C46" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D46" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E46" s="98">
+        <f t="shared" si="6"/>
+        <v>33400</v>
+      </c>
+      <c r="F46" s="101">
+        <f>E46</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B47" s="96">
+        <v>31</v>
+      </c>
+      <c r="C47" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D47" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E47" s="98">
+        <f t="shared" si="6"/>
+        <v>39600</v>
+      </c>
+      <c r="F47" s="101">
+        <f>E46+E47</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B48" s="96">
+        <v>27</v>
+      </c>
+      <c r="C48" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D48" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E48" s="98">
+        <f t="shared" si="6"/>
+        <v>41200</v>
+      </c>
+      <c r="F48" s="101">
+        <f>E46+E47+E48</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B49" s="96">
+        <v>24</v>
+      </c>
+      <c r="C49" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D49" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E49" s="98">
+        <f t="shared" si="6"/>
+        <v>27400</v>
+      </c>
+      <c r="F49" s="102">
+        <f>E49</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B50" s="96">
+        <v>19</v>
+      </c>
+      <c r="C50" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D50" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E50" s="98">
+        <f t="shared" si="6"/>
+        <v>35200</v>
+      </c>
+      <c r="F50" s="102">
+        <f>E49+E50</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B51" s="96">
+        <v>17</v>
+      </c>
+      <c r="C51" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D51" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E51" s="98">
+        <f t="shared" si="6"/>
+        <v>28400</v>
+      </c>
+      <c r="F51" s="102">
+        <f>E49+E50+E51</f>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B52" s="96">
+        <v>13</v>
+      </c>
+      <c r="C52" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D52" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E52" s="98">
+        <f>C52-D52</f>
+        <v>26900</v>
+      </c>
+      <c r="F52" s="99">
+        <f>E52</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B53" s="96">
+        <v>19</v>
+      </c>
+      <c r="C53" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D53" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E53" s="98">
+        <f t="shared" ref="E53:E54" si="7">C53-D53</f>
+        <v>40200</v>
+      </c>
+      <c r="F53" s="99">
+        <f>E52+E53</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B54" s="96">
+        <v>25</v>
+      </c>
+      <c r="C54" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D54" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E54" s="98">
+        <f t="shared" si="7"/>
+        <v>91400</v>
+      </c>
+      <c r="F54" s="99">
+        <f>E52+E53+E54</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B55" s="96">
+        <v>22</v>
+      </c>
+      <c r="C55" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D55" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E55" s="98">
+        <f>C55-D55</f>
+        <v>36300</v>
+      </c>
+      <c r="F55" s="100">
+        <f>E55</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B56" s="96">
+        <v>28</v>
+      </c>
+      <c r="C56" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D56" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E56" s="98">
+        <f t="shared" ref="E56:E63" si="8">C56-D56</f>
+        <v>39700</v>
+      </c>
+      <c r="F56" s="100">
+        <f>E55+E56</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B57" s="96">
+        <v>35</v>
+      </c>
+      <c r="C57" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D57" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E57" s="98">
+        <f t="shared" si="8"/>
+        <v>46200</v>
+      </c>
+      <c r="F57" s="100">
+        <f>E55+E56+E57</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B58" s="96">
+        <v>20</v>
+      </c>
+      <c r="C58" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D58" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E58" s="98">
+        <f t="shared" si="8"/>
+        <v>33400</v>
+      </c>
+      <c r="F58" s="101">
+        <f>E58</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B59" s="96">
+        <v>31</v>
+      </c>
+      <c r="C59" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D59" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E59" s="98">
+        <f t="shared" si="8"/>
+        <v>39600</v>
+      </c>
+      <c r="F59" s="101">
+        <f>E58+E59</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B60" s="96">
+        <v>27</v>
+      </c>
+      <c r="C60" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D60" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E60" s="98">
+        <f t="shared" si="8"/>
+        <v>41200</v>
+      </c>
+      <c r="F60" s="101">
+        <f>E58+E59+E60</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B61" s="96">
+        <v>24</v>
+      </c>
+      <c r="C61" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D61" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E61" s="98">
+        <f t="shared" si="8"/>
+        <v>27400</v>
+      </c>
+      <c r="F61" s="102">
+        <f>E61</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B62" s="96">
+        <v>19</v>
+      </c>
+      <c r="C62" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D62" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E62" s="98">
+        <f t="shared" si="8"/>
+        <v>35200</v>
+      </c>
+      <c r="F62" s="102">
+        <f>E61+E62</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B63" s="96">
+        <v>17</v>
+      </c>
+      <c r="C63" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D63" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E63" s="98">
+        <f t="shared" si="8"/>
+        <v>28400</v>
+      </c>
+      <c r="F63" s="102">
+        <f>E61+E62+E63</f>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B64" s="96">
+        <v>13</v>
+      </c>
+      <c r="C64" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D64" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E64" s="98">
+        <f>C64-D64</f>
+        <v>26900</v>
+      </c>
+      <c r="F64" s="99">
+        <f>E64</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B65" s="96">
+        <v>19</v>
+      </c>
+      <c r="C65" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D65" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E65" s="98">
+        <f t="shared" ref="E65:E66" si="9">C65-D65</f>
+        <v>40200</v>
+      </c>
+      <c r="F65" s="99">
+        <f>E64+E65</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B66" s="96">
+        <v>25</v>
+      </c>
+      <c r="C66" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D66" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E66" s="98">
+        <f t="shared" si="9"/>
+        <v>91400</v>
+      </c>
+      <c r="F66" s="99">
+        <f>E64+E65+E66</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B67" s="96">
+        <v>22</v>
+      </c>
+      <c r="C67" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D67" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E67" s="98">
+        <f>C67-D67</f>
+        <v>36300</v>
+      </c>
+      <c r="F67" s="100">
+        <f>E67</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B68" s="96">
+        <v>28</v>
+      </c>
+      <c r="C68" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D68" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E68" s="98">
+        <f t="shared" ref="E68:E75" si="10">C68-D68</f>
+        <v>39700</v>
+      </c>
+      <c r="F68" s="100">
+        <f>E67+E68</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B69" s="96">
+        <v>35</v>
+      </c>
+      <c r="C69" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D69" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E69" s="98">
+        <f t="shared" si="10"/>
+        <v>46200</v>
+      </c>
+      <c r="F69" s="100">
+        <f>E67+E68+E69</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B70" s="96">
+        <v>20</v>
+      </c>
+      <c r="C70" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D70" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E70" s="98">
+        <f t="shared" si="10"/>
+        <v>33400</v>
+      </c>
+      <c r="F70" s="101">
+        <f>E70</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B71" s="96">
+        <v>31</v>
+      </c>
+      <c r="C71" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D71" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E71" s="98">
+        <f t="shared" si="10"/>
+        <v>39600</v>
+      </c>
+      <c r="F71" s="101">
+        <f>E70+E71</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B72" s="96">
+        <v>27</v>
+      </c>
+      <c r="C72" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D72" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E72" s="98">
+        <f t="shared" si="10"/>
+        <v>41200</v>
+      </c>
+      <c r="F72" s="101">
+        <f>E70+E71+E72</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B73" s="96">
+        <v>24</v>
+      </c>
+      <c r="C73" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D73" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E73" s="98">
+        <f t="shared" si="10"/>
+        <v>27400</v>
+      </c>
+      <c r="F73" s="102">
+        <f>E73</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B74" s="96">
+        <v>19</v>
+      </c>
+      <c r="C74" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D74" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E74" s="98">
+        <f t="shared" si="10"/>
+        <v>35200</v>
+      </c>
+      <c r="F74" s="102">
+        <f>E73+E74</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B75" s="96">
+        <v>17</v>
+      </c>
+      <c r="C75" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D75" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E75" s="98">
+        <f t="shared" si="10"/>
+        <v>28400</v>
+      </c>
+      <c r="F75" s="102">
+        <f>E73+E74+E75</f>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B76" s="96">
+        <v>13</v>
+      </c>
+      <c r="C76" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D76" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E76" s="98">
+        <f>C76-D76</f>
+        <v>26900</v>
+      </c>
+      <c r="F76" s="99">
+        <f>E76</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B77" s="96">
+        <v>19</v>
+      </c>
+      <c r="C77" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D77" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E77" s="98">
+        <f t="shared" ref="E77:E78" si="11">C77-D77</f>
+        <v>40200</v>
+      </c>
+      <c r="F77" s="99">
+        <f>E76+E77</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B78" s="96">
+        <v>25</v>
+      </c>
+      <c r="C78" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D78" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E78" s="98">
+        <f t="shared" si="11"/>
+        <v>91400</v>
+      </c>
+      <c r="F78" s="99">
+        <f>E76+E77+E78</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B79" s="96">
+        <v>22</v>
+      </c>
+      <c r="C79" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D79" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E79" s="98">
+        <f>C79-D79</f>
+        <v>36300</v>
+      </c>
+      <c r="F79" s="100">
+        <f>E79</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B80" s="96">
+        <v>28</v>
+      </c>
+      <c r="C80" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D80" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E80" s="98">
+        <f t="shared" ref="E80:E87" si="12">C80-D80</f>
+        <v>39700</v>
+      </c>
+      <c r="F80" s="100">
+        <f>E79+E80</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B81" s="96">
+        <v>35</v>
+      </c>
+      <c r="C81" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D81" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E81" s="98">
+        <f t="shared" si="12"/>
+        <v>46200</v>
+      </c>
+      <c r="F81" s="100">
+        <f>E79+E80+E81</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A82" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B82" s="96">
+        <v>20</v>
+      </c>
+      <c r="C82" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D82" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E82" s="98">
+        <f t="shared" si="12"/>
+        <v>33400</v>
+      </c>
+      <c r="F82" s="101">
+        <f>E82</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B83" s="96">
+        <v>31</v>
+      </c>
+      <c r="C83" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D83" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E83" s="98">
+        <f t="shared" si="12"/>
+        <v>39600</v>
+      </c>
+      <c r="F83" s="101">
+        <f>E82+E83</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B84" s="96">
+        <v>27</v>
+      </c>
+      <c r="C84" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D84" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E84" s="98">
+        <f t="shared" si="12"/>
+        <v>41200</v>
+      </c>
+      <c r="F84" s="101">
+        <f>E82+E83+E84</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B85" s="96">
+        <v>24</v>
+      </c>
+      <c r="C85" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D85" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E85" s="98">
+        <f t="shared" si="12"/>
+        <v>27400</v>
+      </c>
+      <c r="F85" s="102">
+        <f>E85</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B86" s="96">
+        <v>19</v>
+      </c>
+      <c r="C86" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D86" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E86" s="98">
+        <f t="shared" si="12"/>
+        <v>35200</v>
+      </c>
+      <c r="F86" s="102">
+        <f>E85+E86</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B87" s="96">
+        <v>17</v>
+      </c>
+      <c r="C87" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D87" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E87" s="98">
+        <f t="shared" si="12"/>
+        <v>28400</v>
+      </c>
+      <c r="F87" s="102">
+        <f>E85+E86+E87</f>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B88" s="96">
+        <v>13</v>
+      </c>
+      <c r="C88" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D88" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E88" s="98">
+        <f>C88-D88</f>
+        <v>26900</v>
+      </c>
+      <c r="F88" s="99">
+        <f>E88</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B89" s="96">
+        <v>19</v>
+      </c>
+      <c r="C89" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D89" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E89" s="98">
+        <f t="shared" ref="E89:E90" si="13">C89-D89</f>
+        <v>40200</v>
+      </c>
+      <c r="F89" s="99">
+        <f>E88+E89</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B90" s="96">
+        <v>25</v>
+      </c>
+      <c r="C90" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D90" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E90" s="98">
+        <f t="shared" si="13"/>
+        <v>91400</v>
+      </c>
+      <c r="F90" s="99">
+        <f>E88+E89+E90</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B91" s="96">
+        <v>22</v>
+      </c>
+      <c r="C91" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D91" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E91" s="98">
+        <f>C91-D91</f>
+        <v>36300</v>
+      </c>
+      <c r="F91" s="100">
+        <f>E91</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B92" s="96">
+        <v>28</v>
+      </c>
+      <c r="C92" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D92" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E92" s="98">
+        <f t="shared" ref="E92:E99" si="14">C92-D92</f>
+        <v>39700</v>
+      </c>
+      <c r="F92" s="100">
+        <f>E91+E92</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B93" s="96">
+        <v>35</v>
+      </c>
+      <c r="C93" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D93" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E93" s="98">
+        <f t="shared" si="14"/>
+        <v>46200</v>
+      </c>
+      <c r="F93" s="100">
+        <f>E91+E92+E93</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B94" s="96">
+        <v>20</v>
+      </c>
+      <c r="C94" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D94" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E94" s="98">
+        <f t="shared" si="14"/>
+        <v>33400</v>
+      </c>
+      <c r="F94" s="101">
+        <f>E94</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A95" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B95" s="96">
+        <v>31</v>
+      </c>
+      <c r="C95" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D95" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E95" s="98">
+        <f t="shared" si="14"/>
+        <v>39600</v>
+      </c>
+      <c r="F95" s="101">
+        <f>E94+E95</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B96" s="96">
+        <v>27</v>
+      </c>
+      <c r="C96" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D96" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E96" s="98">
+        <f t="shared" si="14"/>
+        <v>41200</v>
+      </c>
+      <c r="F96" s="101">
+        <f>E94+E95+E96</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B97" s="96">
+        <v>24</v>
+      </c>
+      <c r="C97" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D97" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E97" s="98">
+        <f t="shared" si="14"/>
+        <v>27400</v>
+      </c>
+      <c r="F97" s="102">
+        <f>E97</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B98" s="96">
+        <v>19</v>
+      </c>
+      <c r="C98" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D98" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E98" s="98">
+        <f t="shared" si="14"/>
+        <v>35200</v>
+      </c>
+      <c r="F98" s="102">
+        <f>E97+E98</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A99" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B99" s="96">
+        <v>17</v>
+      </c>
+      <c r="C99" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D99" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E99" s="98">
+        <f t="shared" si="14"/>
+        <v>28400</v>
+      </c>
+      <c r="F99" s="102">
+        <f>E97+E98+E99</f>
+        <v>91000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A100" s="95">
+        <v>42384</v>
+      </c>
+      <c r="B100" s="96">
+        <v>13</v>
+      </c>
+      <c r="C100" s="97">
+        <v>89500</v>
+      </c>
+      <c r="D100" s="97">
+        <v>62600</v>
+      </c>
+      <c r="E100" s="98">
+        <f>C100-D100</f>
+        <v>26900</v>
+      </c>
+      <c r="F100" s="99">
+        <f>E100</f>
+        <v>26900</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="95">
+        <v>42415</v>
+      </c>
+      <c r="B101" s="96">
+        <v>19</v>
+      </c>
+      <c r="C101" s="97">
+        <v>100500</v>
+      </c>
+      <c r="D101" s="97">
+        <v>60300</v>
+      </c>
+      <c r="E101" s="98">
+        <f t="shared" ref="E101:E102" si="15">C101-D101</f>
+        <v>40200</v>
+      </c>
+      <c r="F101" s="99">
+        <f>E100+E101</f>
+        <v>67100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A102" s="95">
+        <v>42444</v>
+      </c>
+      <c r="B102" s="96">
+        <v>25</v>
+      </c>
+      <c r="C102" s="97">
+        <v>119200</v>
+      </c>
+      <c r="D102" s="97">
+        <v>27800</v>
+      </c>
+      <c r="E102" s="98">
+        <f t="shared" si="15"/>
+        <v>91400</v>
+      </c>
+      <c r="F102" s="99">
+        <f>E100+E101+E102</f>
+        <v>158500</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A103" s="95">
+        <v>42475</v>
+      </c>
+      <c r="B103" s="96">
+        <v>22</v>
+      </c>
+      <c r="C103" s="97">
+        <v>115900</v>
+      </c>
+      <c r="D103" s="97">
+        <v>79600</v>
+      </c>
+      <c r="E103" s="98">
+        <f>C103-D103</f>
+        <v>36300</v>
+      </c>
+      <c r="F103" s="100">
+        <f>E103</f>
+        <v>36300</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A104" s="95">
+        <v>42505</v>
+      </c>
+      <c r="B104" s="96">
+        <v>28</v>
+      </c>
+      <c r="C104" s="97">
+        <v>123700</v>
+      </c>
+      <c r="D104" s="97">
+        <v>84000</v>
+      </c>
+      <c r="E104" s="98">
+        <f t="shared" ref="E104:E111" si="16">C104-D104</f>
+        <v>39700</v>
+      </c>
+      <c r="F104" s="100">
+        <f>E103+E104</f>
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A105" s="95">
+        <v>42536</v>
+      </c>
+      <c r="B105" s="96">
+        <v>35</v>
+      </c>
+      <c r="C105" s="97">
+        <v>129300</v>
+      </c>
+      <c r="D105" s="97">
+        <v>83100</v>
+      </c>
+      <c r="E105" s="98">
+        <f t="shared" si="16"/>
+        <v>46200</v>
+      </c>
+      <c r="F105" s="100">
+        <f>E103+E104+E105</f>
+        <v>122200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A106" s="95">
+        <v>42566</v>
+      </c>
+      <c r="B106" s="96">
+        <v>20</v>
+      </c>
+      <c r="C106" s="97">
+        <v>110700</v>
+      </c>
+      <c r="D106" s="97">
+        <v>77300</v>
+      </c>
+      <c r="E106" s="98">
+        <f t="shared" si="16"/>
+        <v>33400</v>
+      </c>
+      <c r="F106" s="101">
+        <f>E106</f>
+        <v>33400</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A107" s="95">
+        <v>42597</v>
+      </c>
+      <c r="B107" s="96">
+        <v>31</v>
+      </c>
+      <c r="C107" s="97">
+        <v>125100</v>
+      </c>
+      <c r="D107" s="97">
+        <v>85500</v>
+      </c>
+      <c r="E107" s="98">
+        <f t="shared" si="16"/>
+        <v>39600</v>
+      </c>
+      <c r="F107" s="101">
+        <f>E106+E107</f>
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A108" s="95">
+        <v>42628</v>
+      </c>
+      <c r="B108" s="96">
+        <v>27</v>
+      </c>
+      <c r="C108" s="97">
+        <v>120100</v>
+      </c>
+      <c r="D108" s="97">
+        <v>78900</v>
+      </c>
+      <c r="E108" s="98">
+        <f t="shared" si="16"/>
+        <v>41200</v>
+      </c>
+      <c r="F108" s="101">
+        <f>E106+E107+E108</f>
+        <v>114200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A109" s="95">
+        <v>42658</v>
+      </c>
+      <c r="B109" s="96">
+        <v>24</v>
+      </c>
+      <c r="C109" s="97">
+        <v>118400</v>
+      </c>
+      <c r="D109" s="97">
+        <v>91000</v>
+      </c>
+      <c r="E109" s="98">
+        <f t="shared" si="16"/>
+        <v>27400</v>
+      </c>
+      <c r="F109" s="102">
+        <f>E109</f>
+        <v>27400</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A110" s="95">
+        <v>42689</v>
+      </c>
+      <c r="B110" s="96">
+        <v>19</v>
+      </c>
+      <c r="C110" s="97">
+        <v>100300</v>
+      </c>
+      <c r="D110" s="97">
+        <v>65100</v>
+      </c>
+      <c r="E110" s="98">
+        <f t="shared" si="16"/>
+        <v>35200</v>
+      </c>
+      <c r="F110" s="102">
+        <f>E109+E110</f>
+        <v>62600</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A111" s="95">
+        <v>42719</v>
+      </c>
+      <c r="B111" s="96">
+        <v>17</v>
+      </c>
+      <c r="C111" s="97">
+        <v>94200</v>
+      </c>
+      <c r="D111" s="97">
+        <v>65800</v>
+      </c>
+      <c r="E111" s="98">
+        <f t="shared" si="16"/>
+        <v>28400</v>
+      </c>
+      <c r="F111" s="102">
+        <f>E109+E110+E111</f>
+        <v>91000</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A3:F15"/>
   <mergeCells count="1">
@@ -17044,6 +19148,86 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C4:C15">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:C27">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28:C39">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:C51">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:C63">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64:C75">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C76:C87">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88:C99">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FFFF7128"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100:C111">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -17589,8 +19773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17763,6 +19947,9 @@
       <c r="D5" s="87">
         <v>3</v>
       </c>
+      <c r="E5" s="87">
+        <v>3</v>
+      </c>
       <c r="G5" s="87">
         <v>3</v>
       </c>
@@ -17775,6 +19962,9 @@
       <c r="J5" s="87">
         <v>3</v>
       </c>
+      <c r="K5" s="87">
+        <v>3</v>
+      </c>
       <c r="M5" s="87">
         <v>3</v>
       </c>
@@ -17785,6 +19975,9 @@
         <v>3</v>
       </c>
       <c r="P5" s="87">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="87">
         <v>3</v>
       </c>
     </row>
@@ -17806,7 +19999,7 @@
       </c>
       <c r="E6" s="87">
         <f>SUBTOTAL(103,Table15[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6" s="87" t="s">
         <v>80</v>
@@ -17825,7 +20018,7 @@
       </c>
       <c r="K6" s="87">
         <f>SUBTOTAL(103,Table16[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6" s="87" t="s">
         <v>80</v>
@@ -17844,7 +20037,7 @@
       </c>
       <c r="Q6" s="87">
         <f>SUBTOTAL(103,Table111[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -18012,6 +20205,9 @@
       <c r="D12" s="87">
         <v>3</v>
       </c>
+      <c r="E12" s="87">
+        <v>3</v>
+      </c>
       <c r="G12" s="87">
         <v>3</v>
       </c>
@@ -18024,6 +20220,9 @@
       <c r="J12" s="87">
         <v>3</v>
       </c>
+      <c r="K12" s="87">
+        <v>3</v>
+      </c>
       <c r="M12" s="87">
         <v>3</v>
       </c>
@@ -18034,6 +20233,9 @@
         <v>3</v>
       </c>
       <c r="P12" s="87">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="87">
         <v>3</v>
       </c>
     </row>
@@ -18055,7 +20257,7 @@
       </c>
       <c r="E13" s="87">
         <f>SUBTOTAL(103,Table17[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G13" s="87" t="s">
         <v>80</v>
@@ -18074,7 +20276,7 @@
       </c>
       <c r="K13" s="87">
         <f>SUBTOTAL(103,Table18[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M13" s="87" t="s">
         <v>80</v>
@@ -18093,7 +20295,7 @@
       </c>
       <c r="Q13" s="87">
         <f>SUBTOTAL(103,Table112[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -18165,6 +20367,9 @@
       <c r="D19" s="87">
         <v>3</v>
       </c>
+      <c r="E19" s="87">
+        <v>3</v>
+      </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="87" t="s">
@@ -18184,7 +20389,7 @@
       </c>
       <c r="E20" s="87">
         <f>SUBTOTAL(103,Table19[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
@@ -18352,6 +20557,9 @@
       <c r="D27" s="87">
         <v>3</v>
       </c>
+      <c r="E27" s="87">
+        <v>3</v>
+      </c>
       <c r="G27" s="87">
         <v>3</v>
       </c>
@@ -18364,6 +20572,9 @@
       <c r="J27" s="87">
         <v>3</v>
       </c>
+      <c r="K27" s="87">
+        <v>3</v>
+      </c>
       <c r="M27" s="87">
         <v>3</v>
       </c>
@@ -18374,6 +20585,9 @@
         <v>3</v>
       </c>
       <c r="P27" s="87">
+        <v>3</v>
+      </c>
+      <c r="Q27" s="87">
         <v>3</v>
       </c>
     </row>
@@ -18395,7 +20609,7 @@
       </c>
       <c r="E28" s="87">
         <f>SUBTOTAL(103,Table1562[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G28" s="87" t="s">
         <v>80</v>
@@ -18414,7 +20628,7 @@
       </c>
       <c r="K28" s="87">
         <f>SUBTOTAL(103,Table1663[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M28" s="87" t="s">
         <v>80</v>
@@ -18433,7 +20647,7 @@
       </c>
       <c r="Q28" s="87">
         <f>SUBTOTAL(103,Table11167[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
@@ -18601,6 +20815,9 @@
       <c r="D34" s="87">
         <v>3</v>
       </c>
+      <c r="E34" s="87">
+        <v>3</v>
+      </c>
       <c r="G34" s="87">
         <v>3</v>
       </c>
@@ -18613,6 +20830,9 @@
       <c r="J34" s="87">
         <v>3</v>
       </c>
+      <c r="K34" s="87">
+        <v>3</v>
+      </c>
       <c r="M34" s="87">
         <v>3</v>
       </c>
@@ -18623,6 +20843,9 @@
         <v>3</v>
       </c>
       <c r="P34" s="87">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="87">
         <v>3</v>
       </c>
     </row>
@@ -18644,7 +20867,7 @@
       </c>
       <c r="E35" s="87">
         <f>SUBTOTAL(103,Table1764[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G35" s="87" t="s">
         <v>80</v>
@@ -18663,7 +20886,7 @@
       </c>
       <c r="K35" s="87">
         <f>SUBTOTAL(103,Table1865[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M35" s="87" t="s">
         <v>80</v>
@@ -18682,7 +20905,7 @@
       </c>
       <c r="Q35" s="87">
         <f>SUBTOTAL(103,Table11268[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -18754,6 +20977,9 @@
       <c r="D41" s="87">
         <v>3</v>
       </c>
+      <c r="E41" s="87">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="87" t="s">
@@ -18773,7 +20999,7 @@
       </c>
       <c r="E42" s="87">
         <f>SUBTOTAL(103,Table1966[Column5])</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a pie chart for a bug fixed
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="5"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="number format" sheetId="9" r:id="rId1"/>
@@ -2156,6 +2156,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2397,11 +2398,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2099154000"/>
-        <c:axId val="-2126315120"/>
+        <c:axId val="-2135007168"/>
+        <c:axId val="-2083872048"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2099154000"/>
+        <c:axId val="-2135007168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2444,7 +2445,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126315120"/>
+        <c:crossAx val="-2083872048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2452,7 +2453,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126315120"/>
+        <c:axId val="-2083872048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2503,7 +2504,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099154000"/>
+        <c:crossAx val="-2135007168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2517,6 +2518,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2598,6 +2600,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2844,11 +2847,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2099143216"/>
-        <c:axId val="-2099139920"/>
+        <c:axId val="2121565552"/>
+        <c:axId val="-2125357664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2099143216"/>
+        <c:axId val="2121565552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2891,7 +2894,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099139920"/>
+        <c:crossAx val="-2125357664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2899,7 +2902,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099139920"/>
+        <c:axId val="-2125357664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2950,7 +2953,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099143216"/>
+        <c:crossAx val="2121565552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2964,6 +2967,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3045,6 +3049,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3291,11 +3296,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2028373024"/>
-        <c:axId val="-2124119536"/>
+        <c:axId val="-2086748608"/>
+        <c:axId val="2071379312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2028373024"/>
+        <c:axId val="-2086748608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3338,7 +3343,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124119536"/>
+        <c:crossAx val="2071379312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3346,7 +3351,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124119536"/>
+        <c:axId val="2071379312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3397,7 +3402,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2028373024"/>
+        <c:crossAx val="-2086748608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3411,6 +3416,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3492,6 +3498,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3794,11 +3801,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="-2099576048"/>
-        <c:axId val="-2099572800"/>
+        <c:axId val="-2091943296"/>
+        <c:axId val="-2091939952"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="-2099576048"/>
+        <c:axId val="-2091943296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3841,12 +3848,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099572800"/>
+        <c:crossAx val="-2091939952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2099572800"/>
+        <c:axId val="-2091939952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3897,7 +3904,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099576048"/>
+        <c:crossAx val="-2091943296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3911,6 +3918,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3992,6 +4000,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4375,6 +4384,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4456,6 +4466,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4710,11 +4721,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2111732720"/>
-        <c:axId val="-2126362800"/>
+        <c:axId val="-2087141680"/>
+        <c:axId val="-2087138384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111732720"/>
+        <c:axId val="-2087141680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4757,7 +4768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2126362800"/>
+        <c:crossAx val="-2087138384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4765,7 +4776,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126362800"/>
+        <c:axId val="-2087138384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4816,7 +4827,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2111732720"/>
+        <c:crossAx val="-2087141680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4830,6 +4841,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4911,6 +4923,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5161,11 +5174,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2122637440"/>
-        <c:axId val="-2122880288"/>
+        <c:axId val="2071204672"/>
+        <c:axId val="2071208240"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2122637440"/>
+        <c:axId val="2071204672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5222,7 +5235,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122880288"/>
+        <c:crossAx val="2071208240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5230,7 +5243,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2122880288"/>
+        <c:axId val="2071208240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5281,7 +5294,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2122637440"/>
+        <c:crossAx val="2071204672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5295,6 +5308,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5376,6 +5390,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5659,11 +5674,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2099558624"/>
-        <c:axId val="-2099555344"/>
+        <c:axId val="-2094561744"/>
+        <c:axId val="-2094716352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2099558624"/>
+        <c:axId val="-2094561744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5720,12 +5735,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099555344"/>
+        <c:crossAx val="-2094716352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2099555344"/>
+        <c:axId val="-2094716352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5776,7 +5791,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099558624"/>
+        <c:crossAx val="-2094561744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5790,6 +5805,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5871,6 +5887,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5901,63 +5918,10 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
-    <c:view3D>
-      <c:rotX val="15"/>
-      <c:rotY val="20"/>
-      <c:rAngAx val="0"/>
-    </c:view3D>
-    <c:floor>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="15000"/>
-              <a:lumOff val="85000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:round/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d contourW="9525">
-          <a:contourClr>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="15000"/>
-              <a:lumOff val="85000"/>
-            </a:schemeClr>
-          </a:contourClr>
-        </a:sp3d>
-      </c:spPr>
-    </c:floor>
-    <c:sideWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:sideWall>
-    <c:backWall>
-      <c:thickness val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-        <a:sp3d/>
-      </c:spPr>
-    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:bar3DChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
-        <c:varyColors val="0"/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -5972,17 +5936,58 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>Charts!$A$2:$A$5</c:f>
@@ -6040,17 +6045,58 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>Charts!$A$2:$A$5</c:f>
@@ -6108,17 +6154,58 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-            <a:sp3d/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:cat>
             <c:numRef>
               <c:f>Charts!$A$2:$A$5</c:f>
@@ -6169,120 +6256,10 @@
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:shape val="box"/>
-        <c:axId val="2028348528"/>
-        <c:axId val="-2122764352"/>
-        <c:axId val="0"/>
-      </c:bar3DChart>
-      <c:catAx>
-        <c:axId val="2028348528"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="-2122764352"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2122764352"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2028348528"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6293,6 +6270,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -19687,8 +19665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19773,7 +19751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add more Chinese number format
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="4"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460"/>
   </bookViews>
   <sheets>
     <sheet name="number format" sheetId="9" r:id="rId1"/>
@@ -537,7 +537,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="27">
+  <numFmts count="29">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
@@ -565,6 +565,8 @@
     <numFmt numFmtId="188" formatCode="00000\-0000"/>
     <numFmt numFmtId="189" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
     <numFmt numFmtId="190" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;"/>
+    <numFmt numFmtId="191" formatCode="[DBNum1][$-404]General"/>
+    <numFmt numFmtId="192" formatCode="[DBNum2][$-404]General"/>
   </numFmts>
   <fonts count="43" x14ac:knownFonts="1">
     <font>
@@ -1185,7 +1187,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1560,6 +1562,8 @@
     <xf numFmtId="188" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="189" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="190" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2156,7 +2160,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2398,11 +2401,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2135007168"/>
-        <c:axId val="-2083872048"/>
+        <c:axId val="-2134874672"/>
+        <c:axId val="-2068297232"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2135007168"/>
+        <c:axId val="-2134874672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2445,7 +2448,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2083872048"/>
+        <c:crossAx val="-2068297232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2453,7 +2456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2083872048"/>
+        <c:axId val="-2068297232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2504,7 +2507,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2135007168"/>
+        <c:crossAx val="-2134874672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2518,7 +2521,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2600,7 +2602,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2847,11 +2848,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121565552"/>
-        <c:axId val="-2125357664"/>
+        <c:axId val="-2071130832"/>
+        <c:axId val="-2071127536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121565552"/>
+        <c:axId val="-2071130832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2894,7 +2895,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2125357664"/>
+        <c:crossAx val="-2071127536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2902,7 +2903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2125357664"/>
+        <c:axId val="-2071127536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2953,7 +2954,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121565552"/>
+        <c:crossAx val="-2071130832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2967,7 +2968,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3049,7 +3049,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3296,11 +3295,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2086748608"/>
-        <c:axId val="2071379312"/>
+        <c:axId val="-2071080432"/>
+        <c:axId val="-2071077136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2086748608"/>
+        <c:axId val="-2071080432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3343,7 +3342,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2071379312"/>
+        <c:crossAx val="-2071077136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3351,7 +3350,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2071379312"/>
+        <c:axId val="-2071077136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3402,7 +3401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2086748608"/>
+        <c:crossAx val="-2071080432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3416,7 +3415,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3498,7 +3496,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3801,11 +3798,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="-2091943296"/>
-        <c:axId val="-2091939952"/>
+        <c:axId val="-2066813408"/>
+        <c:axId val="2054486784"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="-2091943296"/>
+        <c:axId val="-2066813408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3848,12 +3845,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091939952"/>
+        <c:crossAx val="2054486784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2091939952"/>
+        <c:axId val="2054486784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3904,7 +3901,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091943296"/>
+        <c:crossAx val="-2066813408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3918,7 +3915,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4000,7 +3996,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4384,7 +4379,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4466,7 +4460,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4721,11 +4714,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2087141680"/>
-        <c:axId val="-2087138384"/>
+        <c:axId val="-2138371104"/>
+        <c:axId val="-2138142832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087141680"/>
+        <c:axId val="-2138371104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4768,7 +4761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2087138384"/>
+        <c:crossAx val="-2138142832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4776,7 +4769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2087138384"/>
+        <c:axId val="-2138142832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4827,7 +4820,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2087141680"/>
+        <c:crossAx val="-2138371104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4841,7 +4834,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4923,7 +4915,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5174,11 +5165,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2071204672"/>
-        <c:axId val="2071208240"/>
+        <c:axId val="-2138385840"/>
+        <c:axId val="-2138237776"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2071204672"/>
+        <c:axId val="-2138385840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5235,7 +5226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2071208240"/>
+        <c:crossAx val="-2138237776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5243,7 +5234,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2071208240"/>
+        <c:axId val="-2138237776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5294,7 +5285,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2071204672"/>
+        <c:crossAx val="-2138385840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5308,7 +5299,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5390,7 +5380,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5674,11 +5663,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2094561744"/>
-        <c:axId val="-2094716352"/>
+        <c:axId val="-2090296192"/>
+        <c:axId val="-2094740464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2094561744"/>
+        <c:axId val="-2090296192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5735,12 +5724,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094716352"/>
+        <c:crossAx val="-2094740464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094716352"/>
+        <c:axId val="-2094740464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5791,7 +5780,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094561744"/>
+        <c:crossAx val="-2090296192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5805,7 +5794,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5887,7 +5875,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6270,7 +6257,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12164,7 +12150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -12173,8 +12159,8 @@
     <col min="1" max="1" width="29.33203125" style="87" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" style="87" customWidth="1"/>
     <col min="3" max="3" width="30" style="87" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="87" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="87" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38" style="87" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" style="87" customWidth="1"/>
     <col min="6" max="6" width="13.83203125" style="87" customWidth="1"/>
     <col min="7" max="7" width="11" style="87" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="9" style="87"/>
@@ -12199,7 +12185,12 @@
       <c r="C2" s="109">
         <v>-1234.56</v>
       </c>
-      <c r="E2" s="106"/>
+      <c r="D2" s="131">
+        <v>123456789</v>
+      </c>
+      <c r="E2" s="132">
+        <v>9876543</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="105" t="s">
@@ -16706,14 +16697,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="131"/>
-      <c r="C1" s="131"/>
-      <c r="D1" s="131"/>
-      <c r="E1" s="131"/>
-      <c r="F1" s="131"/>
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="133"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="89"/>
@@ -19266,8 +19257,8 @@
         <v>32</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="135"/>
-      <c r="M1" s="135"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -19286,11 +19277,11 @@
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="135" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="133"/>
-      <c r="D3" s="133"/>
+      <c r="C3" s="135"/>
+      <c r="D3" s="135"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -19300,16 +19291,16 @@
         <v>34</v>
       </c>
       <c r="K3" s="9"/>
-      <c r="L3" s="136"/>
-      <c r="M3" s="136"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
-      <c r="B4" s="133" t="s">
+      <c r="B4" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="133"/>
-      <c r="D4" s="133"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="135"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -19319,16 +19310,16 @@
         <v>0</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="L4" s="136"/>
-      <c r="M4" s="136"/>
+      <c r="L4" s="138"/>
+      <c r="M4" s="138"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
-      <c r="B5" s="134" t="s">
+      <c r="B5" s="136" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="134"/>
-      <c r="D5" s="134"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="136"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -19338,8 +19329,8 @@
         <v>1</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
+      <c r="L5" s="138"/>
+      <c r="M5" s="138"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
@@ -19373,10 +19364,10 @@
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="132"/>
+      <c r="C8" s="134"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="18" t="s">
@@ -19665,7 +19656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add more number format
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -42,6 +42,94 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Korea</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Spanish</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Nigeria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Mongolia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>philippines</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>japan</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Windows User</author>
@@ -143,7 +231,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Windows User</author>
@@ -537,7 +625,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="29">
+  <numFmts count="35">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
@@ -567,8 +655,14 @@
     <numFmt numFmtId="190" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;"/>
     <numFmt numFmtId="191" formatCode="[DBNum1][$-404]General"/>
     <numFmt numFmtId="192" formatCode="[DBNum2][$-404]General"/>
+    <numFmt numFmtId="195" formatCode="[$₩-412]#,##0.00"/>
+    <numFmt numFmtId="196" formatCode="[$₡-140A]#,##0.00"/>
+    <numFmt numFmtId="197" formatCode="[$₦-470]\ #,##0.00"/>
+    <numFmt numFmtId="198" formatCode="_-* #,##0.00\ [$₮-450]_-;\-* #,##0.00\ [$₮-450]_-;_-* &quot;-&quot;??\ [$₮-450]_-;_-@_-"/>
+    <numFmt numFmtId="199" formatCode="_([$₱-464]* #,##0.00_);_([$₱-464]* \(#,##0.00\);_([$₱-464]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="200" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
   </numFmts>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -854,8 +948,22 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -907,6 +1015,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF8BBCC7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,7 +1301,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1538,32 +1652,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="171" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="172" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="40" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="173" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="175" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="179" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="181" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="182" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="183" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="184" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="13" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="185" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="186" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="187" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="188" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="189" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="190" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="192" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1587,6 +1677,37 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="171" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="172" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="40" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="191" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="192" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="173" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="174" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="175" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="176" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="179" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="180" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="181" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="182" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="183" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="184" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="13" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="185" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="186" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="187" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="188" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="189" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="195" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="196" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="197" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="198" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="199" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="200" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2401,11 +2522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2134874672"/>
-        <c:axId val="-2068297232"/>
+        <c:axId val="-2146789264"/>
+        <c:axId val="-2146785792"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2134874672"/>
+        <c:axId val="-2146789264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2448,7 +2569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2068297232"/>
+        <c:crossAx val="-2146785792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2456,7 +2577,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2068297232"/>
+        <c:axId val="-2146785792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2507,7 +2628,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2134874672"/>
+        <c:crossAx val="-2146789264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2848,11 +2969,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2071130832"/>
-        <c:axId val="-2071127536"/>
+        <c:axId val="2116194336"/>
+        <c:axId val="2116197664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2071130832"/>
+        <c:axId val="2116194336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2895,7 +3016,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071127536"/>
+        <c:crossAx val="2116197664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2903,7 +3024,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071127536"/>
+        <c:axId val="2116197664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2954,7 +3075,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071130832"/>
+        <c:crossAx val="2116194336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3295,11 +3416,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2071080432"/>
-        <c:axId val="-2071077136"/>
+        <c:axId val="2116141664"/>
+        <c:axId val="2116138256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2071080432"/>
+        <c:axId val="2116141664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3342,7 +3463,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071077136"/>
+        <c:crossAx val="2116138256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3350,7 +3471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2071077136"/>
+        <c:axId val="2116138256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3401,7 +3522,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2071080432"/>
+        <c:crossAx val="2116141664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3798,11 +3919,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="-2066813408"/>
-        <c:axId val="2054486784"/>
+        <c:axId val="2116095824"/>
+        <c:axId val="2116092480"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="-2066813408"/>
+        <c:axId val="2116095824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3845,12 +3966,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2054486784"/>
+        <c:crossAx val="2116092480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2054486784"/>
+        <c:axId val="2116092480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3901,7 +4022,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2066813408"/>
+        <c:crossAx val="2116095824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4714,11 +4835,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2138371104"/>
-        <c:axId val="-2138142832"/>
+        <c:axId val="-2146716224"/>
+        <c:axId val="-2146712832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2138371104"/>
+        <c:axId val="-2146716224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4761,7 +4882,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138142832"/>
+        <c:crossAx val="-2146712832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4769,7 +4890,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138142832"/>
+        <c:axId val="-2146712832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4820,7 +4941,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138371104"/>
+        <c:crossAx val="-2146716224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5165,11 +5286,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2138385840"/>
-        <c:axId val="-2138237776"/>
+        <c:axId val="-2145901424"/>
+        <c:axId val="-2145897808"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2138385840"/>
+        <c:axId val="-2145901424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5226,7 +5347,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138237776"/>
+        <c:crossAx val="-2145897808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5234,7 +5355,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2138237776"/>
+        <c:axId val="-2145897808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5285,7 +5406,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2138385840"/>
+        <c:crossAx val="-2145901424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5663,11 +5784,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2090296192"/>
-        <c:axId val="-2094740464"/>
+        <c:axId val="-2146651408"/>
+        <c:axId val="-2146648112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2090296192"/>
+        <c:axId val="-2146651408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5724,12 +5845,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094740464"/>
+        <c:crossAx val="-2146648112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2094740464"/>
+        <c:axId val="-2146648112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5780,7 +5901,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2090296192"/>
+        <c:crossAx val="-2146651408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12147,12 +12268,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12166,8 +12285,8 @@
     <col min="8" max="16384" width="9" style="87"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="105" t="s">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="139" t="s">
         <v>92</v>
       </c>
       <c r="B1" s="106"/>
@@ -12176,24 +12295,24 @@
       <c r="E1" s="106"/>
     </row>
     <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="107">
+      <c r="A2" s="115">
         <v>9.1234567890123408</v>
       </c>
-      <c r="B2" s="108">
+      <c r="B2" s="116">
         <v>-1234.56</v>
       </c>
-      <c r="C2" s="109">
+      <c r="C2" s="117">
         <v>-1234.56</v>
       </c>
-      <c r="D2" s="131">
+      <c r="D2" s="118">
         <v>123456789</v>
       </c>
-      <c r="E2" s="132">
+      <c r="E2" s="119">
         <v>9876543</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="105" t="s">
+    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="139" t="s">
         <v>93</v>
       </c>
       <c r="B3" s="106"/>
@@ -12202,18 +12321,24 @@
       <c r="E3" s="106"/>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="110">
+      <c r="A4" s="120">
         <v>1234.56</v>
       </c>
-      <c r="B4" s="111">
+      <c r="B4" s="121">
         <v>-1234.56</v>
       </c>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-    </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="105" t="s">
+      <c r="C4" s="140">
+        <v>1234.56</v>
+      </c>
+      <c r="D4" s="141">
+        <v>1234.56</v>
+      </c>
+      <c r="E4" s="142">
+        <v>1234.56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A5" s="139" t="s">
         <v>94</v>
       </c>
       <c r="B5" s="106"/>
@@ -12222,20 +12347,24 @@
       <c r="E5" s="106"/>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="112">
+      <c r="A6" s="122">
         <v>1234</v>
       </c>
-      <c r="B6" s="113">
+      <c r="B6" s="123">
         <v>5678</v>
       </c>
-      <c r="C6" s="114">
+      <c r="C6" s="124">
         <v>5678</v>
       </c>
-      <c r="D6" s="106"/>
-      <c r="E6" s="106"/>
-    </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="105" t="s">
+      <c r="D6" s="143">
+        <v>5678</v>
+      </c>
+      <c r="E6" s="144">
+        <v>5678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A7" s="139" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="106"/>
@@ -12244,22 +12373,22 @@
       <c r="E7" s="106"/>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="115">
+      <c r="A8" s="125">
         <v>43202</v>
       </c>
-      <c r="B8" s="116">
+      <c r="B8" s="126">
         <v>43202</v>
       </c>
-      <c r="C8" s="117">
+      <c r="C8" s="127">
         <v>43202</v>
       </c>
-      <c r="D8" s="118">
+      <c r="D8" s="128">
         <v>43202</v>
       </c>
       <c r="E8" s="106"/>
     </row>
-    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="105" t="s">
+    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A9" s="139" t="s">
         <v>96</v>
       </c>
       <c r="B9" s="106"/>
@@ -12268,18 +12397,20 @@
       <c r="E9" s="106"/>
     </row>
     <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="119">
+      <c r="A10" s="129">
         <v>41376</v>
       </c>
-      <c r="B10" s="120">
+      <c r="B10" s="130">
         <v>80808.006192129629</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="106"/>
+      <c r="C10" s="145">
+        <v>80808.006192129629</v>
+      </c>
+      <c r="D10"/>
       <c r="E10" s="106"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="105" t="s">
+    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A11" s="139" t="s">
         <v>97</v>
       </c>
       <c r="B11" s="106"/>
@@ -12288,18 +12419,18 @@
       <c r="E11" s="106"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="121">
+      <c r="A12" s="131">
         <v>0.1234</v>
       </c>
-      <c r="B12" s="122">
+      <c r="B12" s="132">
         <v>0.12345678</v>
       </c>
       <c r="C12" s="106"/>
       <c r="D12" s="106"/>
       <c r="E12" s="106"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="105" t="s">
+    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A13" s="139" t="s">
         <v>98</v>
       </c>
       <c r="B13" s="106"/>
@@ -12308,18 +12439,18 @@
       <c r="E13" s="106"/>
     </row>
     <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="123">
+      <c r="A14" s="133">
         <v>0.48</v>
       </c>
-      <c r="B14" s="124">
+      <c r="B14" s="134">
         <v>0.48399999999999999</v>
       </c>
       <c r="C14" s="106"/>
       <c r="D14" s="106"/>
       <c r="E14" s="106"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="105" t="s">
+    <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A15" s="139" t="s">
         <v>99</v>
       </c>
       <c r="B15" s="106"/>
@@ -12328,18 +12459,18 @@
       <c r="E15" s="106"/>
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="125">
+      <c r="A16" s="135">
         <v>1000000000</v>
       </c>
-      <c r="B16" s="126">
+      <c r="B16" s="136">
         <v>1234000000</v>
       </c>
       <c r="C16" s="106"/>
       <c r="D16" s="106"/>
       <c r="E16" s="106"/>
     </row>
-    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="105" t="s">
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A17" s="139" t="s">
         <v>100</v>
       </c>
       <c r="B17" s="106"/>
@@ -12348,7 +12479,7 @@
       <c r="E17" s="106"/>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="127" t="s">
+      <c r="A18" s="107" t="s">
         <v>101</v>
       </c>
       <c r="B18" s="106"/>
@@ -12356,8 +12487,8 @@
       <c r="D18" s="106"/>
       <c r="E18" s="106"/>
     </row>
-    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="105" t="s">
+    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A19" s="139" t="s">
         <v>102</v>
       </c>
       <c r="B19" s="106"/>
@@ -12366,10 +12497,10 @@
       <c r="E19" s="106"/>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="128">
+      <c r="A20" s="137">
         <v>123456789</v>
       </c>
-      <c r="B20" s="129">
+      <c r="B20" s="138">
         <v>73504450</v>
       </c>
       <c r="C20" s="106"/>
@@ -12384,7 +12515,7 @@
       <c r="E21" s="106"/>
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="130"/>
+      <c r="A22" s="108"/>
       <c r="B22" s="106"/>
       <c r="C22" s="106"/>
       <c r="D22" s="106"/>
@@ -12400,6 +12531,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -16697,14 +16829,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="133"/>
-      <c r="E1" s="133"/>
-      <c r="F1" s="133"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="89"/>
@@ -19257,8 +19389,8 @@
         <v>32</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="137"/>
-      <c r="M1" s="137"/>
+      <c r="L1" s="113"/>
+      <c r="M1" s="113"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -19277,11 +19409,11 @@
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="135" t="s">
+      <c r="B3" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="135"/>
-      <c r="D3" s="135"/>
+      <c r="C3" s="111"/>
+      <c r="D3" s="111"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -19291,16 +19423,16 @@
         <v>34</v>
       </c>
       <c r="K3" s="9"/>
-      <c r="L3" s="138"/>
-      <c r="M3" s="138"/>
+      <c r="L3" s="114"/>
+      <c r="M3" s="114"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="135"/>
-      <c r="D4" s="135"/>
+      <c r="C4" s="111"/>
+      <c r="D4" s="111"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -19310,16 +19442,16 @@
         <v>0</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="L4" s="138"/>
-      <c r="M4" s="138"/>
+      <c r="L4" s="114"/>
+      <c r="M4" s="114"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="136"/>
-      <c r="D5" s="136"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -19329,8 +19461,8 @@
         <v>1</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="138"/>
-      <c r="M5" s="138"/>
+      <c r="L5" s="114"/>
+      <c r="M5" s="114"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
@@ -19364,10 +19496,10 @@
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
-      <c r="B8" s="134" t="s">
+      <c r="B8" s="110" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="134"/>
+      <c r="C8" s="110"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="18" t="s">

</xml_diff>

<commit_message>
add text rotation sheet
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/java-client-demo/src/main/webapp/book/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/java-client-demo/src/main/webapp/book/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,17 +13,18 @@
   </bookViews>
   <sheets>
     <sheet name="number format" sheetId="9" r:id="rId1"/>
-    <sheet name="conditionalFormatting" sheetId="5" r:id="rId2"/>
-    <sheet name="filter" sheetId="6" r:id="rId3"/>
-    <sheet name="validation" sheetId="1" r:id="rId4"/>
-    <sheet name="Charts" sheetId="7" r:id="rId5"/>
-    <sheet name="TableStyle" sheetId="8" r:id="rId6"/>
-    <sheet name="protection" sheetId="4" r:id="rId7"/>
-    <sheet name="source" sheetId="2" r:id="rId8"/>
+    <sheet name="rotation" sheetId="10" r:id="rId2"/>
+    <sheet name="conditionalFormatting" sheetId="5" r:id="rId3"/>
+    <sheet name="filter" sheetId="6" r:id="rId4"/>
+    <sheet name="validation" sheetId="1" r:id="rId5"/>
+    <sheet name="Charts" sheetId="7" r:id="rId6"/>
+    <sheet name="TableStyle" sheetId="8" r:id="rId7"/>
+    <sheet name="protection" sheetId="4" r:id="rId8"/>
+    <sheet name="source" sheetId="2" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">filter!$A$3:$F$15</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">protection!$A$1:$F$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">filter!$A$3:$F$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="7">protection!$A$1:$F$9</definedName>
     <definedName name="RangeMerged">'number format'!$F$8</definedName>
     <definedName name="SourceItems">source!$B$11:$B$20</definedName>
     <definedName name="TestRange1">'number format'!$D$8:$D$17</definedName>
@@ -267,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="111">
   <si>
     <t>Big City, YA</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -620,6 +621,32 @@
   <si>
     <t>special (phone)</t>
   </si>
+  <si>
+    <t>Text Rotation Degrees</t>
+  </si>
+  <si>
+    <t>Vertical Bottom</t>
+  </si>
+  <si>
+    <t>Apple
+Banana Cake
+Dragon</t>
+  </si>
+  <si>
+    <t>Vertical Center</t>
+  </si>
+  <si>
+    <t>Vertical Top</t>
+  </si>
+  <si>
+    <t>Horizontal Left</t>
+  </si>
+  <si>
+    <t>Horizontal Center</t>
+  </si>
+  <si>
+    <t>Horizontal Right</t>
+  </si>
 </sst>
 </file>
 
@@ -662,7 +689,7 @@
     <numFmt numFmtId="197" formatCode="_([$₱-464]* #,##0.00_);_([$₱-464]* \(#,##0.00\);_([$₱-464]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="198" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
   </numFmts>
-  <fonts count="45" x14ac:knownFonts="1">
+  <fonts count="46" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -961,6 +988,14 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1277,7 +1312,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1300,8 +1335,9 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1684,6 +1720,157 @@
     <xf numFmtId="196" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="197" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="198" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="15" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="75" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="15" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="75" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="15" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="75" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="15" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="75" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="15" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="75" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="15" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="30" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="60" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="75" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1707,9 +1894,134 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="105" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="105" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="105" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="105" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="105" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="105" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="91" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="91" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="91" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="91" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="91" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="91" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="120" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="120" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="120" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="120" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="120" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="120" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="135" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="135" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="135" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="135" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="135" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="135" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="140" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="140" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="140" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="140" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="140" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="140" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="165" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="165" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="165" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="165" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="165" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="165" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="11">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
@@ -1720,6 +2032,7 @@
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 3" xfId="3"/>
     <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 5" xfId="10"/>
   </cellStyles>
   <dxfs count="74">
     <dxf>
@@ -2281,6 +2594,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2522,11 +2836,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2099566192"/>
-        <c:axId val="-2077760304"/>
+        <c:axId val="-2114407760"/>
+        <c:axId val="-2114404464"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2099566192"/>
+        <c:axId val="-2114407760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2569,7 +2883,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2077760304"/>
+        <c:crossAx val="-2114404464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2577,7 +2891,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077760304"/>
+        <c:axId val="-2114404464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2628,7 +2942,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099566192"/>
+        <c:crossAx val="-2114407760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2642,6 +2956,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2723,6 +3038,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2969,11 +3285,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2117306160"/>
-        <c:axId val="-2114458480"/>
+        <c:axId val="-2119082416"/>
+        <c:axId val="-2119063888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2117306160"/>
+        <c:axId val="-2119082416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3016,7 +3332,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114458480"/>
+        <c:crossAx val="-2119063888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3024,7 +3340,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114458480"/>
+        <c:axId val="-2119063888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3075,7 +3391,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117306160"/>
+        <c:crossAx val="-2119082416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3089,6 +3405,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3170,6 +3487,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3416,11 +3734,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2114683904"/>
-        <c:axId val="-2097449664"/>
+        <c:axId val="-2124664016"/>
+        <c:axId val="2077804304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2114683904"/>
+        <c:axId val="-2124664016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3463,7 +3781,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097449664"/>
+        <c:crossAx val="2077804304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3471,7 +3789,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097449664"/>
+        <c:axId val="2077804304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3522,7 +3840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114683904"/>
+        <c:crossAx val="-2124664016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3536,6 +3854,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3617,6 +3936,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3919,11 +4239,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="-2097697200"/>
-        <c:axId val="-2078801680"/>
+        <c:axId val="2076336448"/>
+        <c:axId val="2131648016"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="-2097697200"/>
+        <c:axId val="2076336448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3966,12 +4286,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078801680"/>
+        <c:crossAx val="2131648016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2078801680"/>
+        <c:axId val="2131648016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4022,7 +4342,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097697200"/>
+        <c:crossAx val="2076336448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4036,6 +4356,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4117,6 +4438,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4500,6 +4822,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4581,6 +4904,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4835,11 +5159,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2076588656"/>
-        <c:axId val="2117364080"/>
+        <c:axId val="2090242416"/>
+        <c:axId val="2127775296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2076588656"/>
+        <c:axId val="2090242416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4882,7 +5206,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117364080"/>
+        <c:crossAx val="2127775296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4890,7 +5214,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117364080"/>
+        <c:axId val="2127775296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4941,7 +5265,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2076588656"/>
+        <c:crossAx val="2090242416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4955,6 +5279,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5036,6 +5361,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5286,11 +5612,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2098680480"/>
-        <c:axId val="-2098517024"/>
+        <c:axId val="-2129116432"/>
+        <c:axId val="-2129112864"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2098680480"/>
+        <c:axId val="-2129116432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5347,7 +5673,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098517024"/>
+        <c:crossAx val="-2129112864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5355,7 +5681,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2098517024"/>
+        <c:axId val="-2129112864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5406,7 +5732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2098680480"/>
+        <c:crossAx val="-2129116432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5420,6 +5746,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5501,6 +5828,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5784,11 +6112,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2114865792"/>
-        <c:axId val="-2078463856"/>
+        <c:axId val="-2123441184"/>
+        <c:axId val="-2123437904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2114865792"/>
+        <c:axId val="-2123441184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5845,12 +6173,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2078463856"/>
+        <c:crossAx val="-2123437904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2078463856"/>
+        <c:axId val="-2123437904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5901,7 +6229,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114865792"/>
+        <c:crossAx val="-2123441184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5915,6 +6243,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5996,6 +6325,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6378,6 +6708,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12272,7 +12603,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12481,7 +12812,7 @@
       <c r="E17" s="106"/>
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="145" t="s">
+      <c r="A18" s="139" t="s">
         <v>101</v>
       </c>
       <c r="B18" s="106"/>
@@ -12538,6 +12869,376 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" style="141" customWidth="1"/>
+    <col min="2" max="16" width="17.1640625" style="141" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="141"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="140" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="141">
+        <v>0</v>
+      </c>
+      <c r="C1" s="141">
+        <v>1</v>
+      </c>
+      <c r="D1" s="141">
+        <v>15</v>
+      </c>
+      <c r="E1" s="141">
+        <v>30</v>
+      </c>
+      <c r="F1" s="141">
+        <v>45</v>
+      </c>
+      <c r="G1" s="141">
+        <v>60</v>
+      </c>
+      <c r="H1" s="141">
+        <v>75</v>
+      </c>
+      <c r="I1" s="141">
+        <v>90</v>
+      </c>
+      <c r="J1" s="141">
+        <v>-1</v>
+      </c>
+      <c r="K1" s="141">
+        <v>-15</v>
+      </c>
+      <c r="L1" s="141">
+        <v>-30</v>
+      </c>
+      <c r="M1" s="141">
+        <v>-45</v>
+      </c>
+      <c r="N1" s="141">
+        <v>-60</v>
+      </c>
+      <c r="O1" s="141">
+        <v>-75</v>
+      </c>
+      <c r="P1" s="141">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="140" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="142" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="143" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="144" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="145" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="146" t="s">
+        <v>105</v>
+      </c>
+      <c r="G2" s="147" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="148" t="s">
+        <v>105</v>
+      </c>
+      <c r="I2" s="149" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" s="202" t="s">
+        <v>105</v>
+      </c>
+      <c r="K2" s="196" t="s">
+        <v>105</v>
+      </c>
+      <c r="L2" s="208" t="s">
+        <v>105</v>
+      </c>
+      <c r="M2" s="214" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" s="220" t="s">
+        <v>105</v>
+      </c>
+      <c r="O2" s="226" t="s">
+        <v>105</v>
+      </c>
+      <c r="P2" s="232" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="140" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3" s="150" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="151" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="152" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="153" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" s="154" t="s">
+        <v>105</v>
+      </c>
+      <c r="G3" s="155" t="s">
+        <v>105</v>
+      </c>
+      <c r="H3" s="156" t="s">
+        <v>105</v>
+      </c>
+      <c r="I3" s="157" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="203" t="s">
+        <v>105</v>
+      </c>
+      <c r="K3" s="197" t="s">
+        <v>105</v>
+      </c>
+      <c r="L3" s="209" t="s">
+        <v>105</v>
+      </c>
+      <c r="M3" s="215" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="221" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" s="227" t="s">
+        <v>105</v>
+      </c>
+      <c r="P3" s="233" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="140" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="158" t="s">
+        <v>105</v>
+      </c>
+      <c r="C4" s="159" t="s">
+        <v>105</v>
+      </c>
+      <c r="D4" s="160" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="161" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="162" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="163" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="164" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" s="165" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="204" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" s="198" t="s">
+        <v>105</v>
+      </c>
+      <c r="L4" s="210" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="216" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" s="222" t="s">
+        <v>105</v>
+      </c>
+      <c r="O4" s="228" t="s">
+        <v>105</v>
+      </c>
+      <c r="P4" s="234" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="140" t="s">
+        <v>108</v>
+      </c>
+      <c r="B5" s="166" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5" s="167" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="168" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="169" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" s="170" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" s="171" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="172" t="s">
+        <v>105</v>
+      </c>
+      <c r="I5" s="173" t="s">
+        <v>105</v>
+      </c>
+      <c r="J5" s="205" t="s">
+        <v>105</v>
+      </c>
+      <c r="K5" s="199" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" s="211" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5" s="217" t="s">
+        <v>105</v>
+      </c>
+      <c r="N5" s="223" t="s">
+        <v>105</v>
+      </c>
+      <c r="O5" s="229" t="s">
+        <v>105</v>
+      </c>
+      <c r="P5" s="235" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="140" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="174" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="175" t="s">
+        <v>105</v>
+      </c>
+      <c r="D6" s="176" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="177" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="178" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="179" t="s">
+        <v>105</v>
+      </c>
+      <c r="H6" s="180" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="181" t="s">
+        <v>105</v>
+      </c>
+      <c r="J6" s="206" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="200" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" s="212" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" s="218" t="s">
+        <v>105</v>
+      </c>
+      <c r="N6" s="224" t="s">
+        <v>105</v>
+      </c>
+      <c r="O6" s="230" t="s">
+        <v>105</v>
+      </c>
+      <c r="P6" s="236" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="140" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="182" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="183" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" s="184" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="185" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="186" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" s="187" t="s">
+        <v>105</v>
+      </c>
+      <c r="H7" s="188" t="s">
+        <v>105</v>
+      </c>
+      <c r="I7" s="189" t="s">
+        <v>105</v>
+      </c>
+      <c r="J7" s="207" t="s">
+        <v>105</v>
+      </c>
+      <c r="K7" s="201" t="s">
+        <v>105</v>
+      </c>
+      <c r="L7" s="213" t="s">
+        <v>105</v>
+      </c>
+      <c r="M7" s="219" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" s="225" t="s">
+        <v>105</v>
+      </c>
+      <c r="O7" s="231" t="s">
+        <v>105</v>
+      </c>
+      <c r="P7" s="237" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M88"/>
   <sheetViews>
@@ -16811,7 +17512,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F111"/>
   <sheetViews>
@@ -16831,14 +17532,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="190" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
+      <c r="B1" s="190"/>
+      <c r="C1" s="190"/>
+      <c r="D1" s="190"/>
+      <c r="E1" s="190"/>
+      <c r="F1" s="190"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="89"/>
@@ -19350,7 +20051,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M20"/>
   <sheetViews>
@@ -19391,8 +20092,8 @@
         <v>32</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="143"/>
-      <c r="M1" s="143"/>
+      <c r="L1" s="194"/>
+      <c r="M1" s="194"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -19411,11 +20112,11 @@
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="192" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="141"/>
+      <c r="C3" s="192"/>
+      <c r="D3" s="192"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -19425,16 +20126,16 @@
         <v>34</v>
       </c>
       <c r="K3" s="9"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
+      <c r="L3" s="195"/>
+      <c r="M3" s="195"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
-      <c r="B4" s="141" t="s">
+      <c r="B4" s="192" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
+      <c r="C4" s="192"/>
+      <c r="D4" s="192"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -19444,16 +20145,16 @@
         <v>0</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="L4" s="144"/>
-      <c r="M4" s="144"/>
+      <c r="L4" s="195"/>
+      <c r="M4" s="195"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
-      <c r="B5" s="142" t="s">
+      <c r="B5" s="193" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="142"/>
-      <c r="D5" s="142"/>
+      <c r="C5" s="193"/>
+      <c r="D5" s="193"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -19463,8 +20164,8 @@
         <v>1</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="144"/>
+      <c r="L5" s="195"/>
+      <c r="M5" s="195"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
@@ -19498,10 +20199,10 @@
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="191" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="140"/>
+      <c r="C8" s="191"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="18" t="s">
@@ -19786,7 +20487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -19872,7 +20573,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q42"/>
   <sheetViews>
@@ -21126,7 +21827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor indexed="26"/>
@@ -21284,7 +21985,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J22"/>
   <sheetViews>

</xml_diff>

<commit_message>
add a sheet for "text rotation"
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="number format" sheetId="9" r:id="rId1"/>
-    <sheet name="rotation" sheetId="10" r:id="rId2"/>
+    <sheet name="rotation" sheetId="11" r:id="rId2"/>
     <sheet name="conditionalFormatting" sheetId="5" r:id="rId3"/>
     <sheet name="filter" sheetId="6" r:id="rId4"/>
     <sheet name="validation" sheetId="1" r:id="rId5"/>
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="111">
   <si>
     <t>Big City, YA</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -1337,7 +1337,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="238">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1731,12 +1731,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment textRotation="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment textRotation="15" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment textRotation="30" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
@@ -1749,16 +1743,7 @@
       <alignment textRotation="75" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="center" textRotation="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="center" textRotation="15" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment vertical="center" textRotation="30" wrapText="1"/>
@@ -1773,16 +1758,7 @@
       <alignment vertical="center" textRotation="75" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="top" textRotation="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="top" textRotation="15" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment vertical="top" textRotation="30" wrapText="1"/>
@@ -1797,16 +1773,7 @@
       <alignment vertical="top" textRotation="75" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="top" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="15" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="30" wrapText="1"/>
@@ -1821,16 +1788,7 @@
       <alignment horizontal="left" vertical="center" textRotation="75" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="15" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="30" wrapText="1"/>
@@ -1845,16 +1803,7 @@
       <alignment horizontal="center" vertical="center" textRotation="75" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="1" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="15" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="30" wrapText="1"/>
@@ -1867,50 +1816,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="75" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment textRotation="105" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="center" textRotation="105" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="top" textRotation="105" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="105" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="105" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="105" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment textRotation="91" wrapText="1"/>
@@ -1967,24 +1872,6 @@
       <alignment horizontal="right" vertical="center" textRotation="135" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment textRotation="140" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="center" textRotation="140" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment vertical="top" textRotation="140" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="140" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="140" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="140" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment textRotation="165" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
@@ -2019,6 +1906,47 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment textRotation="150" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="center" textRotation="150" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment vertical="top" textRotation="150" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="150" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="150" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="150" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -2836,11 +2764,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2114407760"/>
-        <c:axId val="-2114404464"/>
+        <c:axId val="2136068784"/>
+        <c:axId val="2136065376"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="-2114407760"/>
+        <c:axId val="2136068784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2883,7 +2811,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114404464"/>
+        <c:crossAx val="2136065376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2891,7 +2819,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2114404464"/>
+        <c:axId val="2136065376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2942,7 +2870,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2114407760"/>
+        <c:crossAx val="2136068784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3285,11 +3213,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2119082416"/>
-        <c:axId val="-2119063888"/>
+        <c:axId val="2137689424"/>
+        <c:axId val="2137692816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2119082416"/>
+        <c:axId val="2137689424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3332,7 +3260,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119063888"/>
+        <c:crossAx val="2137692816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3340,7 +3268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2119063888"/>
+        <c:axId val="2137692816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3391,7 +3319,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2119082416"/>
+        <c:crossAx val="2137689424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3734,11 +3662,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2124664016"/>
-        <c:axId val="2077804304"/>
+        <c:axId val="2138906256"/>
+        <c:axId val="2138909648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2124664016"/>
+        <c:axId val="2138906256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3781,7 +3709,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2077804304"/>
+        <c:crossAx val="2138909648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3789,7 +3717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2077804304"/>
+        <c:axId val="2138909648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3840,7 +3768,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2124664016"/>
+        <c:crossAx val="2138906256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4239,11 +4167,11 @@
         </c:dLbls>
         <c:bubbleScale val="100"/>
         <c:showNegBubbles val="0"/>
-        <c:axId val="2076336448"/>
-        <c:axId val="2131648016"/>
+        <c:axId val="-2129162144"/>
+        <c:axId val="-2129158800"/>
       </c:bubbleChart>
       <c:valAx>
-        <c:axId val="2076336448"/>
+        <c:axId val="-2129162144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4286,12 +4214,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2131648016"/>
+        <c:crossAx val="-2129158800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2131648016"/>
+        <c:axId val="-2129158800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4342,7 +4270,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2076336448"/>
+        <c:crossAx val="-2129162144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5159,11 +5087,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2090242416"/>
-        <c:axId val="2127775296"/>
+        <c:axId val="2139017664"/>
+        <c:axId val="2139021056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2090242416"/>
+        <c:axId val="2139017664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5206,7 +5134,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2127775296"/>
+        <c:crossAx val="2139021056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5214,7 +5142,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127775296"/>
+        <c:axId val="2139021056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5265,7 +5193,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2090242416"/>
+        <c:crossAx val="2139017664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5612,11 +5540,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2129116432"/>
-        <c:axId val="-2129112864"/>
+        <c:axId val="-2129129840"/>
+        <c:axId val="-2129126224"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2129116432"/>
+        <c:axId val="-2129129840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5673,7 +5601,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129112864"/>
+        <c:crossAx val="-2129126224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5681,7 +5609,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2129112864"/>
+        <c:axId val="-2129126224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5732,7 +5660,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2129116432"/>
+        <c:crossAx val="-2129129840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6112,11 +6040,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2123441184"/>
-        <c:axId val="-2123437904"/>
+        <c:axId val="2138927280"/>
+        <c:axId val="2139031744"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2123441184"/>
+        <c:axId val="2138927280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6173,12 +6101,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123437904"/>
+        <c:crossAx val="2139031744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2123437904"/>
+        <c:axId val="2139031744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6229,7 +6157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2123441184"/>
+        <c:crossAx val="2138927280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12602,9 +12530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12870,20 +12796,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="141" customWidth="1"/>
-    <col min="2" max="16" width="17.1640625" style="141" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="141"/>
+    <col min="1" max="1" width="11.33203125" style="141" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" style="141" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="141" customWidth="1"/>
+    <col min="4" max="7" width="17.1640625" style="141" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" style="141" customWidth="1"/>
+    <col min="9" max="12" width="17.1640625" style="141" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="141"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A1" s="140" t="s">
         <v>103</v>
       </c>
@@ -12891,49 +12821,37 @@
         <v>0</v>
       </c>
       <c r="C1" s="141">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D1" s="141">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="E1" s="141">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F1" s="141">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="G1" s="141">
-        <v>60</v>
+        <v>-1</v>
       </c>
       <c r="H1" s="141">
-        <v>75</v>
+        <v>-30</v>
       </c>
       <c r="I1" s="141">
-        <v>90</v>
+        <v>-45</v>
       </c>
       <c r="J1" s="141">
-        <v>-1</v>
+        <v>-60</v>
       </c>
       <c r="K1" s="141">
-        <v>-15</v>
+        <v>-75</v>
       </c>
       <c r="L1" s="141">
-        <v>-30</v>
-      </c>
-      <c r="M1" s="141">
-        <v>-45</v>
-      </c>
-      <c r="N1" s="141">
-        <v>-60</v>
-      </c>
-      <c r="O1" s="141">
-        <v>-75</v>
-      </c>
-      <c r="P1" s="141">
         <v>-90</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="140" t="s">
         <v>104</v>
       </c>
@@ -12952,260 +12870,200 @@
       <c r="F2" s="146" t="s">
         <v>105</v>
       </c>
-      <c r="G2" s="147" t="s">
+      <c r="G2" s="172" t="s">
         <v>105</v>
       </c>
-      <c r="H2" s="148" t="s">
+      <c r="H2" s="178" t="s">
         <v>105</v>
       </c>
-      <c r="I2" s="149" t="s">
+      <c r="I2" s="184" t="s">
         <v>105</v>
       </c>
       <c r="J2" s="202" t="s">
         <v>105</v>
       </c>
-      <c r="K2" s="196" t="s">
+      <c r="K2" s="190" t="s">
         <v>105</v>
       </c>
-      <c r="L2" s="208" t="s">
+      <c r="L2" s="196" t="s">
         <v>105</v>
       </c>
-      <c r="M2" s="214" t="s">
-        <v>105</v>
-      </c>
-      <c r="N2" s="220" t="s">
-        <v>105</v>
-      </c>
-      <c r="O2" s="226" t="s">
-        <v>105</v>
-      </c>
-      <c r="P2" s="232" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="140" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="150" t="s">
+      <c r="B3" s="147" t="s">
         <v>105</v>
       </c>
-      <c r="C3" s="151" t="s">
+      <c r="C3" s="148" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="152" t="s">
+      <c r="D3" s="149" t="s">
         <v>105</v>
       </c>
-      <c r="E3" s="153" t="s">
+      <c r="E3" s="150" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="154" t="s">
+      <c r="F3" s="151" t="s">
         <v>105</v>
       </c>
-      <c r="G3" s="155" t="s">
+      <c r="G3" s="173" t="s">
         <v>105</v>
       </c>
-      <c r="H3" s="156" t="s">
+      <c r="H3" s="179" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="157" t="s">
+      <c r="I3" s="185" t="s">
         <v>105</v>
       </c>
       <c r="J3" s="203" t="s">
         <v>105</v>
       </c>
-      <c r="K3" s="197" t="s">
+      <c r="K3" s="191" t="s">
         <v>105</v>
       </c>
-      <c r="L3" s="209" t="s">
+      <c r="L3" s="197" t="s">
         <v>105</v>
       </c>
-      <c r="M3" s="215" t="s">
-        <v>105</v>
-      </c>
-      <c r="N3" s="221" t="s">
-        <v>105</v>
-      </c>
-      <c r="O3" s="227" t="s">
-        <v>105</v>
-      </c>
-      <c r="P3" s="233" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="140" t="s">
         <v>107</v>
       </c>
-      <c r="B4" s="158" t="s">
+      <c r="B4" s="152" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="159" t="s">
+      <c r="C4" s="153" t="s">
         <v>105</v>
       </c>
-      <c r="D4" s="160" t="s">
+      <c r="D4" s="154" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="161" t="s">
+      <c r="E4" s="155" t="s">
         <v>105</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="156" t="s">
         <v>105</v>
       </c>
-      <c r="G4" s="163" t="s">
+      <c r="G4" s="174" t="s">
         <v>105</v>
       </c>
-      <c r="H4" s="164" t="s">
+      <c r="H4" s="180" t="s">
         <v>105</v>
       </c>
-      <c r="I4" s="165" t="s">
+      <c r="I4" s="186" t="s">
         <v>105</v>
       </c>
       <c r="J4" s="204" t="s">
         <v>105</v>
       </c>
-      <c r="K4" s="198" t="s">
+      <c r="K4" s="192" t="s">
         <v>105</v>
       </c>
-      <c r="L4" s="210" t="s">
+      <c r="L4" s="198" t="s">
         <v>105</v>
       </c>
-      <c r="M4" s="216" t="s">
-        <v>105</v>
-      </c>
-      <c r="N4" s="222" t="s">
-        <v>105</v>
-      </c>
-      <c r="O4" s="228" t="s">
-        <v>105</v>
-      </c>
-      <c r="P4" s="234" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="140" t="s">
         <v>108</v>
       </c>
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="157" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="167" t="s">
+      <c r="C5" s="158" t="s">
         <v>105</v>
       </c>
-      <c r="D5" s="168" t="s">
+      <c r="D5" s="159" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="169" t="s">
+      <c r="E5" s="160" t="s">
         <v>105</v>
       </c>
-      <c r="F5" s="170" t="s">
+      <c r="F5" s="161" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="171" t="s">
+      <c r="G5" s="175" t="s">
         <v>105</v>
       </c>
-      <c r="H5" s="172" t="s">
+      <c r="H5" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="I5" s="173" t="s">
+      <c r="I5" s="187" t="s">
         <v>105</v>
       </c>
       <c r="J5" s="205" t="s">
         <v>105</v>
       </c>
-      <c r="K5" s="199" t="s">
+      <c r="K5" s="193" t="s">
         <v>105</v>
       </c>
-      <c r="L5" s="211" t="s">
+      <c r="L5" s="199" t="s">
         <v>105</v>
       </c>
-      <c r="M5" s="217" t="s">
-        <v>105</v>
-      </c>
-      <c r="N5" s="223" t="s">
-        <v>105</v>
-      </c>
-      <c r="O5" s="229" t="s">
-        <v>105</v>
-      </c>
-      <c r="P5" s="235" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="140" t="s">
         <v>109</v>
       </c>
-      <c r="B6" s="174" t="s">
+      <c r="B6" s="162" t="s">
         <v>105</v>
       </c>
-      <c r="C6" s="175" t="s">
+      <c r="C6" s="163" t="s">
         <v>105</v>
       </c>
-      <c r="D6" s="176" t="s">
+      <c r="D6" s="164" t="s">
         <v>105</v>
       </c>
-      <c r="E6" s="177" t="s">
+      <c r="E6" s="165" t="s">
         <v>105</v>
       </c>
-      <c r="F6" s="178" t="s">
+      <c r="F6" s="166" t="s">
         <v>105</v>
       </c>
-      <c r="G6" s="179" t="s">
+      <c r="G6" s="176" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="180" t="s">
+      <c r="H6" s="182" t="s">
         <v>105</v>
       </c>
-      <c r="I6" s="181" t="s">
+      <c r="I6" s="188" t="s">
         <v>105</v>
       </c>
       <c r="J6" s="206" t="s">
         <v>105</v>
       </c>
-      <c r="K6" s="200" t="s">
+      <c r="K6" s="194" t="s">
         <v>105</v>
       </c>
-      <c r="L6" s="212" t="s">
+      <c r="L6" s="200" t="s">
         <v>105</v>
       </c>
-      <c r="M6" s="218" t="s">
-        <v>105</v>
-      </c>
-      <c r="N6" s="224" t="s">
-        <v>105</v>
-      </c>
-      <c r="O6" s="230" t="s">
-        <v>105</v>
-      </c>
-      <c r="P6" s="236" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="140" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="182" t="s">
+      <c r="B7" s="167" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="183" t="s">
+      <c r="C7" s="168" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="184" t="s">
+      <c r="D7" s="169" t="s">
         <v>105</v>
       </c>
-      <c r="E7" s="185" t="s">
+      <c r="E7" s="170" t="s">
         <v>105</v>
       </c>
-      <c r="F7" s="186" t="s">
+      <c r="F7" s="171" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="187" t="s">
+      <c r="G7" s="177" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="188" t="s">
+      <c r="H7" s="183" t="s">
         <v>105</v>
       </c>
       <c r="I7" s="189" t="s">
@@ -13214,22 +13072,10 @@
       <c r="J7" s="207" t="s">
         <v>105</v>
       </c>
-      <c r="K7" s="201" t="s">
+      <c r="K7" s="195" t="s">
         <v>105</v>
       </c>
-      <c r="L7" s="213" t="s">
-        <v>105</v>
-      </c>
-      <c r="M7" s="219" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" s="225" t="s">
-        <v>105</v>
-      </c>
-      <c r="O7" s="231" t="s">
-        <v>105</v>
-      </c>
-      <c r="P7" s="237" t="s">
+      <c r="L7" s="201" t="s">
         <v>105</v>
       </c>
     </row>
@@ -13242,8 +13088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M88"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17517,7 +17363,7 @@
   <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17532,14 +17378,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="190" t="s">
+      <c r="A1" s="208" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="190"/>
-      <c r="C1" s="190"/>
-      <c r="D1" s="190"/>
-      <c r="E1" s="190"/>
-      <c r="F1" s="190"/>
+      <c r="B1" s="208"/>
+      <c r="C1" s="208"/>
+      <c r="D1" s="208"/>
+      <c r="E1" s="208"/>
+      <c r="F1" s="208"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="89"/>
@@ -20092,8 +19938,8 @@
         <v>32</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="194"/>
-      <c r="M1" s="194"/>
+      <c r="L1" s="212"/>
+      <c r="M1" s="212"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -20112,11 +19958,11 @@
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="192" t="s">
+      <c r="B3" s="210" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="192"/>
-      <c r="D3" s="192"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -20126,16 +19972,16 @@
         <v>34</v>
       </c>
       <c r="K3" s="9"/>
-      <c r="L3" s="195"/>
-      <c r="M3" s="195"/>
+      <c r="L3" s="213"/>
+      <c r="M3" s="213"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
-      <c r="B4" s="192" t="s">
+      <c r="B4" s="210" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="192"/>
-      <c r="D4" s="192"/>
+      <c r="C4" s="210"/>
+      <c r="D4" s="210"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -20145,16 +19991,16 @@
         <v>0</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="L4" s="195"/>
-      <c r="M4" s="195"/>
+      <c r="L4" s="213"/>
+      <c r="M4" s="213"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
-      <c r="B5" s="193" t="s">
+      <c r="B5" s="211" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="193"/>
-      <c r="D5" s="193"/>
+      <c r="C5" s="211"/>
+      <c r="D5" s="211"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -20164,8 +20010,8 @@
         <v>1</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="195"/>
-      <c r="M5" s="195"/>
+      <c r="L5" s="213"/>
+      <c r="M5" s="213"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
@@ -20199,10 +20045,10 @@
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
-      <c r="B8" s="191" t="s">
+      <c r="B8" s="209" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="191"/>
+      <c r="C8" s="209"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="18" t="s">

</xml_diff>

<commit_message>
add more number, date format
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/java-client-demo/src/main/webapp/book/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A103201-CE0B-0E47-B8E1-470C10576B3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="number format" sheetId="9" r:id="rId1"/>
@@ -22,15 +23,23 @@
     <sheet name="protection" sheetId="4" r:id="rId8"/>
     <sheet name="source" sheetId="2" r:id="rId9"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId10"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">filter!$A$3:$F$15</definedName>
+    <definedName name="CalendarMonth">IF(Month="January",1,IF(Month="February",2,IF(Month="March",3,IF(Month="April",4,IF(Month="May",5,IF(Month="June",6,IF(Month="July",7,IF(Month="August",8,IF(Month="September",9,IF(Month="October",10,IF(Month="November",11,12)))))))))))</definedName>
+    <definedName name="CalendarYear">#REF!</definedName>
+    <definedName name="DueDate">#REF!</definedName>
+    <definedName name="Month">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">protection!$A$1:$F$9</definedName>
-    <definedName name="RangeMerged">'number format'!$F$8</definedName>
+    <definedName name="RangeMerged">'number format'!$F$9</definedName>
     <definedName name="SourceItems">source!$B$11:$B$20</definedName>
-    <definedName name="TestRange1">'number format'!$D$8:$D$17</definedName>
-    <definedName name="TestRange2">'number format'!$F$8</definedName>
+    <definedName name="TestRange1">'number format'!$D$9:$D$20</definedName>
+    <definedName name="TestRange2">'number format'!$F$9</definedName>
+    <definedName name="TransplantDate">'[1]Seed Starting Log'!$G$3</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -43,12 +52,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="C4" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,12 +65,27 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>Korea</t>
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Spanish</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -69,12 +93,27 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
-          <t>Spanish</t>
+          <t>Nigeria</t>
         </r>
       </text>
     </comment>
-    <comment ref="E4" authorId="0">
+    <comment ref="D7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mongolia</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -82,45 +121,21 @@
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
-          <t>Nigeria</t>
+          <t>philippines</t>
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
-          </rPr>
-          <t>Mongolia</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E6" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
-          </rPr>
-          <t>philippines</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C10" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri"/>
+            <family val="2"/>
           </rPr>
           <t>japan</t>
         </r>
@@ -131,12 +146,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -144,6 +159,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Windows User:</t>
         </r>
@@ -152,6 +168,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 revenue
@@ -159,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0">
+    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -167,6 +184,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Windows User:</t>
         </r>
@@ -175,6 +193,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 revenue
@@ -182,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A39" authorId="0">
+    <comment ref="A39" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -190,6 +209,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Windows User:</t>
         </r>
@@ -198,6 +218,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 revenue
@@ -205,7 +226,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A59" authorId="0">
+    <comment ref="A59" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -213,6 +234,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>Windows User:</t>
         </r>
@@ -221,6 +243,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 revenue
@@ -233,30 +256,32 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="I8" authorId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t>The discount should no be greater than 5%.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">The date should not be later than the current date.
 </t>
@@ -651,8 +676,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="35">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="48">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
@@ -688,8 +713,21 @@
     <numFmt numFmtId="196" formatCode="_-* #,##0.00\ [$₮-450]_-;\-* #,##0.00\ [$₮-450]_-;_-* &quot;-&quot;??\ [$₮-450]_-;_-@_-"/>
     <numFmt numFmtId="197" formatCode="_([$₱-464]* #,##0.00_);_([$₱-464]* \(#,##0.00\);_([$₱-464]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="198" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
+    <numFmt numFmtId="201" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="202" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="203" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="204" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="205" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="206" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="207" formatCode="[$-409]mmmmm;@"/>
+    <numFmt numFmtId="208" formatCode="[$-409]mmmmm\-yy;@"/>
+    <numFmt numFmtId="210" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="212" formatCode="*0###"/>
+    <numFmt numFmtId="215" formatCode="###* ###"/>
+    <numFmt numFmtId="217" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="218" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
-  <fonts count="46" x14ac:knownFonts="1">
+  <fonts count="51" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -877,10 +915,12 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -917,6 +957,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -988,6 +1029,7 @@
       <sz val="10"/>
       <color indexed="81"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -996,6 +1038,41 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1312,7 +1389,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1336,8 +1413,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="49" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1948,8 +2031,26 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="201" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="202" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="203" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="204" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="205" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="206" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="207" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="208" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="210" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="212" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="215" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="191" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="217" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="218" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
@@ -1957,12 +2058,16 @@
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="3"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normal 5" xfId="10"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 5" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 6" xfId="11" xr:uid="{9237AD53-8488-9247-9944-795A91209C1F}"/>
+    <cellStyle name="Percent 2" xfId="14" xr:uid="{290F6D1A-7A63-434A-86C1-FBE7A45819C2}"/>
+    <cellStyle name="Tip" xfId="13" xr:uid="{512ACF74-4F3A-4849-A93F-FDAB4B380597}"/>
+    <cellStyle name="Title 2" xfId="12" xr:uid="{F938F036-88DA-D841-ABFF-6719FC63356A}"/>
   </cellStyles>
-  <dxfs count="74">
+  <dxfs count="82">
     <dxf>
       <fill>
         <patternFill>
@@ -2481,8 +2586,131 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <vertical style="medium">
+          <color theme="0"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <vertical style="medium">
+          <color theme="0"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Garden Journal: Basic Table" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="81"/>
+      <tableStyleElement type="headerRow" dxfId="80"/>
+      <tableStyleElement type="totalRow" dxfId="79"/>
+      <tableStyleElement type="firstColumn" dxfId="78"/>
+    </tableStyle>
+    <tableStyle name="Garden Journal: Basic Table 2" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="wholeTable" dxfId="77"/>
+      <tableStyleElement type="headerRow" dxfId="76"/>
+      <tableStyleElement type="totalRow" dxfId="75"/>
+      <tableStyleElement type="firstColumn" dxfId="74"/>
+    </tableStyle>
+  </tableStyles>
   <colors>
     <mruColors>
       <color rgb="FFCCE6D0"/>
@@ -2508,7 +2736,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2522,7 +2750,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2588,16 +2815,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2609,20 +2836,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AF63-FA4C-A648-7BF2DBC70F16}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2654,16 +2886,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2675,20 +2907,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AF63-FA4C-A648-7BF2DBC70F16}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2720,16 +2957,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2741,20 +2978,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AF63-FA4C-A648-7BF2DBC70F16}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2884,7 +3126,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2952,7 +3193,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2966,7 +3207,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3034,16 +3274,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3055,20 +3295,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9BCD-1448-B741-48CEB4619563}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3101,16 +3346,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3122,20 +3367,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9BCD-1448-B741-48CEB4619563}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3168,16 +3418,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3189,20 +3439,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9BCD-1448-B741-48CEB4619563}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3333,7 +3588,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3401,7 +3655,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3415,7 +3669,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3483,16 +3736,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3504,20 +3757,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B7F1-2941-A3DA-977985B45774}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3550,16 +3808,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3571,20 +3829,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B7F1-2941-A3DA-977985B45774}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3617,16 +3880,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3638,20 +3901,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B7F1-2941-A3DA-977985B45774}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3782,7 +4050,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3850,7 +4117,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3864,7 +4131,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3930,16 +4196,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3951,16 +4217,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3970,20 +4236,25 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="4"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:bubbleSize>
           <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4D93-CF49-BD15-1C9E9CDED73F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4016,16 +4287,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4037,16 +4308,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4056,20 +4327,25 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="4"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:bubbleSize>
           <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4D93-CF49-BD15-1C9E9CDED73F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4102,16 +4378,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4123,16 +4399,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4142,20 +4418,25 @@
               <c:formatCode>General</c:formatCode>
               <c:ptCount val="4"/>
               <c:pt idx="0">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>1.0</c:v>
+                <c:v>1</c:v>
               </c:pt>
             </c:numLit>
           </c:bubbleSize>
           <c:bubble3D val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4D93-CF49-BD15-1C9E9CDED73F}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4284,7 +4565,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4352,7 +4632,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4366,7 +4646,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4427,6 +4706,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4440,6 +4724,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4453,6 +4742,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -4466,6 +4760,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
@@ -4474,16 +4773,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4495,20 +4794,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-D9DD-BC42-92BC-BC5887A0CF14}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4536,6 +4840,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4549,6 +4858,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4562,6 +4876,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -4575,6 +4894,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
@@ -4583,16 +4907,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4604,20 +4928,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-D9DD-BC42-92BC-BC5887A0CF14}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -4645,6 +4974,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -4658,6 +4992,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -4671,6 +5010,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -4684,6 +5028,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-D9DD-BC42-92BC-BC5887A0CF14}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
@@ -4692,16 +5041,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4713,20 +5062,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001A-D9DD-BC42-92BC-BC5887A0CF14}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -4750,7 +5104,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4818,7 +5171,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4832,7 +5185,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4901,16 +5253,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4922,21 +5274,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-286C-6D44-B50F-6EAAF0FEA687}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -4971,16 +5328,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4992,21 +5349,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-286C-6D44-B50F-6EAAF0FEA687}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5041,16 +5403,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5062,21 +5424,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-286C-6D44-B50F-6EAAF0FEA687}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5207,7 +5574,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5275,7 +5641,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5289,7 +5655,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5358,16 +5723,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5379,20 +5744,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2695-0A46-BFCD-3409A937B143}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5427,16 +5797,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5448,20 +5818,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2695-0A46-BFCD-3409A937B143}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5496,16 +5871,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5517,20 +5892,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-2695-0A46-BFCD-3409A937B143}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -5674,7 +6054,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5742,7 +6121,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -5756,7 +6135,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5835,16 +6213,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5856,21 +6234,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D5C2-3943-89D9-AB293130B384}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -5915,16 +6298,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5936,21 +6319,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D5C2-3943-89D9-AB293130B384}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -5995,16 +6383,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6016,21 +6404,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D5C2-3943-89D9-AB293130B384}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6171,7 +6564,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6239,7 +6631,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -6253,7 +6645,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6314,6 +6705,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -6327,6 +6723,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -6340,6 +6741,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -6353,6 +6759,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
@@ -6361,16 +6772,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6382,20 +6793,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-BC8D-4143-A3A5-7E5D462344FA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -6423,6 +6839,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000A-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -6436,6 +6857,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000C-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -6449,6 +6875,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -6462,6 +6893,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000010-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
@@ -6470,16 +6906,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6491,20 +6927,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000011-BC8D-4143-A3A5-7E5D462344FA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -6532,6 +6973,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000013-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -6545,6 +6991,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000015-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -6558,6 +7009,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000017-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -6571,6 +7027,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000019-BC8D-4143-A3A5-7E5D462344FA}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:numRef>
@@ -6579,16 +7040,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6600,20 +7061,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9.0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000001A-BC8D-4143-A3A5-7E5D462344FA}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -6636,7 +7102,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11769,7 +12234,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11801,7 +12272,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11833,7 +12310,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11865,7 +12348,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11897,7 +12386,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11929,7 +12424,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11961,7 +12462,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvPr id="8" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -11993,7 +12500,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -12025,7 +12538,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvPr id="10" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -12045,197 +12564,222 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Plant Inventory"/>
+      <sheetName val="Seed Starting Log"/>
+      <sheetName val="Task List"/>
+      <sheetName val="Garden Planning Grid"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="G3" t="str">
+            <v>[Date]</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table15" displayName="Table15" ref="A2:E6" totalsRowCount="1">
-  <autoFilter ref="A2:E5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table15" displayName="Table15" ref="A2:E6" totalsRowCount="1">
+  <autoFilter ref="A2:E5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table1764" displayName="Table1764" ref="A31:E35" totalsRowCount="1">
-  <autoFilter ref="A31:E34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="Table1764" displayName="Table1764" ref="A31:E35" totalsRowCount="1">
+  <autoFilter ref="A31:E34" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1865" displayName="Table1865" ref="G31:K35" totalsRowCount="1">
-  <autoFilter ref="G31:K34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="Table1865" displayName="Table1865" ref="G31:K35" totalsRowCount="1">
+  <autoFilter ref="G31:K34" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table1966" displayName="Table1966" ref="A38:E42" totalsRowCount="1">
-  <autoFilter ref="A38:E41"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="Table1966" displayName="Table1966" ref="A38:E42" totalsRowCount="1">
+  <autoFilter ref="A38:E41" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table11167" displayName="Table11167" ref="M24:Q28" totalsRowCount="1">
-  <autoFilter ref="M24:Q27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="Table11167" displayName="Table11167" ref="M24:Q28" totalsRowCount="1">
+  <autoFilter ref="M24:Q27" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0C00-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table11268" displayName="Table11268" ref="M31:Q35" totalsRowCount="1">
-  <autoFilter ref="M31:Q34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="Table11268" displayName="Table11268" ref="M31:Q35" totalsRowCount="1">
+  <autoFilter ref="M31:Q34" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0D00-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table16" displayName="Table16" ref="G2:K6" totalsRowCount="1">
-  <autoFilter ref="G2:K5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table16" displayName="Table16" ref="G2:K6" totalsRowCount="1">
+  <autoFilter ref="G2:K5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table17" displayName="Table17" ref="A9:E13" totalsRowCount="1">
-  <autoFilter ref="A9:E12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table17" displayName="Table17" ref="A9:E13" totalsRowCount="1">
+  <autoFilter ref="A9:E12" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table18" displayName="Table18" ref="G9:K13" totalsRowCount="1">
-  <autoFilter ref="G9:K12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table18" displayName="Table18" ref="G9:K13" totalsRowCount="1">
+  <autoFilter ref="G9:K12" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table19" displayName="Table19" ref="A16:E20" totalsRowCount="1">
-  <autoFilter ref="A16:E19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table19" displayName="Table19" ref="A16:E20" totalsRowCount="1">
+  <autoFilter ref="A16:E19" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table111" displayName="Table111" ref="M2:Q6" totalsRowCount="1">
-  <autoFilter ref="M2:Q5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table111" displayName="Table111" ref="M2:Q6" totalsRowCount="1">
+  <autoFilter ref="M2:Q5" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table112" displayName="Table112" ref="M9:Q13" totalsRowCount="1">
-  <autoFilter ref="M9:Q12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table112" displayName="Table112" ref="M9:Q13" totalsRowCount="1">
+  <autoFilter ref="M9:Q12" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table1562" displayName="Table1562" ref="A24:E28" totalsRowCount="1">
-  <autoFilter ref="A24:E27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table1562" displayName="Table1562" ref="A24:E28" totalsRowCount="1">
+  <autoFilter ref="A24:E27" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table1663" displayName="Table1663" ref="G24:K28" totalsRowCount="1">
-  <autoFilter ref="G24:K27"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="Table1663" displayName="Table1663" ref="G24:K28" totalsRowCount="1">
+  <autoFilter ref="G24:K27" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
-    <tableColumn id="2" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="3" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="4" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
-    <tableColumn id="5" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="Column1" totalsRowLabel="Total" dataCellStyle="Normal 3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="Column2" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="Column3" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="Column4" totalsRowFunction="average" dataCellStyle="Normal 3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="Column5" totalsRowFunction="count" dataCellStyle="Normal 3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -12527,10 +13071,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12570,222 +13116,276 @@
         <v>9876543</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A3" s="132" t="s">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="225">
+        <v>12345.678</v>
+      </c>
+      <c r="B3" s="226">
+        <v>12345</v>
+      </c>
+      <c r="C3" s="226"/>
+      <c r="D3" s="227"/>
+      <c r="E3" s="112"/>
+    </row>
+    <row r="4" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A4" s="132" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-    </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="113">
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="113">
         <v>1234.56</v>
       </c>
-      <c r="B4" s="114">
+      <c r="B5" s="114">
         <v>-1234.56</v>
       </c>
-      <c r="C4" s="133">
+      <c r="C5" s="133">
         <v>1234.56</v>
       </c>
-      <c r="D4" s="134">
+      <c r="D5" s="134">
         <v>1234.56</v>
       </c>
-      <c r="E4" s="135">
+      <c r="E5" s="135">
         <v>1234.56</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A5" s="132" t="s">
+    <row r="6" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A6" s="132" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-    </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="115">
+      <c r="B6" s="106"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="106"/>
+      <c r="E6" s="106"/>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="115">
         <v>1234</v>
       </c>
-      <c r="B6" s="116">
+      <c r="B7" s="116">
         <v>5678</v>
       </c>
-      <c r="C6" s="117">
+      <c r="C7" s="117">
         <v>5678</v>
       </c>
-      <c r="D6" s="136">
+      <c r="D7" s="136">
         <v>5678</v>
       </c>
-      <c r="E6" s="137">
+      <c r="E7" s="137">
         <v>5678</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A7" s="132" t="s">
+    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="132" t="s">
         <v>95</v>
       </c>
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-    </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="118">
+      <c r="B8" s="106"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
+      <c r="E8" s="106"/>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="118">
         <v>43202</v>
       </c>
-      <c r="B8" s="119">
+      <c r="B9" s="119">
         <v>43202</v>
       </c>
-      <c r="C8" s="120">
+      <c r="C9" s="214">
         <v>43202</v>
       </c>
-      <c r="D8" s="121">
+      <c r="D9" s="215">
         <v>43202</v>
       </c>
-      <c r="E8" s="106"/>
-    </row>
-    <row r="9" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A9" s="132" t="s">
+      <c r="E9" s="216">
+        <v>43202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="217">
+        <v>43202</v>
+      </c>
+      <c r="B10" s="218">
+        <v>43202</v>
+      </c>
+      <c r="C10" s="219">
+        <v>43202</v>
+      </c>
+      <c r="D10" s="220">
+        <v>43202</v>
+      </c>
+      <c r="E10" s="121">
+        <v>43202</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="221">
+        <v>43202</v>
+      </c>
+      <c r="B11" s="222">
+        <v>43202</v>
+      </c>
+      <c r="C11" s="223">
+        <v>43202</v>
+      </c>
+      <c r="D11" s="224">
+        <v>43202</v>
+      </c>
+      <c r="E11" s="120">
+        <v>43202</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A12" s="132" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="106"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="106"/>
-      <c r="E9" s="106"/>
-    </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="122">
-        <v>41376</v>
-      </c>
-      <c r="B10" s="123">
-        <v>80808.006192129629</v>
-      </c>
-      <c r="C10" s="138">
-        <v>80808.006192129629</v>
-      </c>
-      <c r="D10"/>
-      <c r="E10" s="106"/>
-    </row>
-    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A11" s="132" t="s">
-        <v>97</v>
-      </c>
-      <c r="B11" s="106"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="106"/>
-      <c r="E11" s="106"/>
-    </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="124">
-        <v>0.1234</v>
-      </c>
-      <c r="B12" s="125">
-        <v>0.12345678</v>
-      </c>
+      <c r="B12" s="106"/>
       <c r="C12" s="106"/>
       <c r="D12" s="106"/>
       <c r="E12" s="106"/>
     </row>
-    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A13" s="132" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="106"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-    </row>
-    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="126">
-        <v>0.48</v>
-      </c>
-      <c r="B14" s="127">
-        <v>0.48399999999999999</v>
-      </c>
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="122">
+        <v>41376</v>
+      </c>
+      <c r="B13" s="123">
+        <v>80808.006192129629</v>
+      </c>
+      <c r="C13" s="138">
+        <v>80808.006192129629</v>
+      </c>
+      <c r="D13" s="228">
+        <v>80808.006192129629</v>
+      </c>
+      <c r="E13" s="229">
+        <v>80808.006192129629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A14" s="132" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="106"/>
       <c r="C14" s="106"/>
       <c r="D14" s="106"/>
       <c r="E14" s="106"/>
     </row>
-    <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A15" s="132" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" s="106"/>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="124">
+        <v>0.1234</v>
+      </c>
+      <c r="B15" s="125">
+        <v>0.12345678</v>
+      </c>
       <c r="C15" s="106"/>
       <c r="D15" s="106"/>
       <c r="E15" s="106"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="128">
-        <v>1000000000</v>
-      </c>
-      <c r="B16" s="129">
-        <v>1234000000</v>
-      </c>
+    <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A16" s="132" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" s="106"/>
       <c r="C16" s="106"/>
       <c r="D16" s="106"/>
       <c r="E16" s="106"/>
     </row>
-    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A17" s="132" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="106"/>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="126">
+        <v>0.48</v>
+      </c>
+      <c r="B17" s="127">
+        <v>0.48399999999999999</v>
+      </c>
       <c r="C17" s="106"/>
       <c r="D17" s="106"/>
       <c r="E17" s="106"/>
     </row>
-    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="139" t="s">
-        <v>101</v>
+    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A18" s="132" t="s">
+        <v>99</v>
       </c>
       <c r="B18" s="106"/>
       <c r="C18" s="106"/>
       <c r="D18" s="106"/>
       <c r="E18" s="106"/>
     </row>
-    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A19" s="132" t="s">
-        <v>102</v>
-      </c>
-      <c r="B19" s="106"/>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="128">
+        <v>1000000000</v>
+      </c>
+      <c r="B19" s="129">
+        <v>1234000000</v>
+      </c>
       <c r="C19" s="106"/>
       <c r="D19" s="106"/>
       <c r="E19" s="106"/>
     </row>
-    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="130">
-        <v>123456789</v>
-      </c>
-      <c r="B20" s="131">
-        <v>73504450</v>
-      </c>
+    <row r="20" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A20" s="132" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="106"/>
       <c r="C20" s="106"/>
       <c r="D20" s="106"/>
       <c r="E20" s="106"/>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="105"/>
+      <c r="A21" s="139" t="s">
+        <v>101</v>
+      </c>
       <c r="B21" s="106"/>
       <c r="C21" s="106"/>
       <c r="D21" s="106"/>
       <c r="E21" s="106"/>
     </row>
-    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A22" s="107"/>
+    <row r="22" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A22" s="132" t="s">
+        <v>102</v>
+      </c>
       <c r="B22" s="106"/>
       <c r="C22" s="106"/>
       <c r="D22" s="106"/>
       <c r="E22" s="106"/>
     </row>
     <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="106"/>
-      <c r="B23" s="106"/>
+      <c r="A23" s="130">
+        <v>123456789</v>
+      </c>
+      <c r="B23" s="131">
+        <v>73504450</v>
+      </c>
       <c r="C23" s="106"/>
       <c r="D23" s="106"/>
       <c r="E23" s="106"/>
+    </row>
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A24" s="105"/>
+      <c r="B24" s="106"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="106"/>
+      <c r="E24" s="106"/>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A25" s="107"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="106"/>
+      <c r="E25" s="106"/>
+    </row>
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="106"/>
+      <c r="B26" s="106"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
+      <c r="E26" s="106"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12795,7 +13395,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12813,7 +13413,7 @@
     <col min="13" max="16384" width="9" style="141"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="48" x14ac:dyDescent="0.2">
       <c r="A1" s="140" t="s">
         <v>103</v>
       </c>
@@ -13085,7 +13685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17359,7 +17959,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F111"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
@@ -19792,7 +20392,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:F15"/>
+  <autoFilter ref="A3:F15" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
@@ -19888,7 +20488,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L11" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>$N$11</formula1>
     </dataValidation>
   </dataValidations>
@@ -19898,7 +20498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
@@ -20310,20 +20910,20 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"30 days,60 days"</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter the discount no greater than 5%." sqref="I10:I13">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter the discount no greater than 5%." sqref="I10:I13" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>0</formula1>
       <formula2>0.05</formula2>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G13">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G13" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The date should not be later than the current date." sqref="C11">
+    <dataValidation type="date" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="The date should not be later than the current date." sqref="C11" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>TODAY()</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F13" xr:uid="{00000000-0002-0000-0400-000004000000}">
       <formula1>SourceItems</formula1>
     </dataValidation>
   </dataValidations>
@@ -20334,7 +20934,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20420,7 +21020,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
@@ -21674,8 +22274,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
     <tabColor indexed="26"/>
   </sheetPr>
   <dimension ref="A1:G11"/>
@@ -21832,7 +22432,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:J22"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">

</xml_diff>

<commit_message>
increase days dropdown column width
</commit_message>
<xml_diff>
--- a/src/main/webapp/book/demo/featuresCompatibility.xlsx
+++ b/src/main/webapp/book/demo/featuresCompatibility.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/java-client-demo/src/main/webapp/book/demo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/keikai-zk/src/main/webapp/book/demo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA50E924-754E-C740-B0EC-F9E21FE64172}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A0CCCA-8077-4543-97AE-DBED69644748}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30400" yWindow="460" windowWidth="33600" windowHeight="20460" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="number format" sheetId="9" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <definedName name="TestRange2">'number format'!$F$9</definedName>
     <definedName name="TransplantDate">'[1]Seed Starting Log'!$G$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -678,54 +678,54 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="48">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="167" formatCode="m/d;@"/>
-    <numFmt numFmtId="168" formatCode="h:mm;@"/>
-    <numFmt numFmtId="169" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="171" formatCode="0.000000000000000"/>
-    <numFmt numFmtId="172" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="173" formatCode="&quot;NT$&quot;#,##0.00"/>
-    <numFmt numFmtId="174" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="175" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_(&quot;US$&quot;* #,##0.00_);_(&quot;US$&quot;* \(#,##0.00\);_(&quot;US$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="178" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="179" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="180" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="181" formatCode="h:mm:ss;@"/>
-    <numFmt numFmtId="182" formatCode="0.0%"/>
-    <numFmt numFmtId="183" formatCode="0.000000%"/>
-    <numFmt numFmtId="184" formatCode="#\ ???/???"/>
-    <numFmt numFmtId="185" formatCode="0.E+00"/>
-    <numFmt numFmtId="186" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="187" formatCode="00000\-0000"/>
-    <numFmt numFmtId="188" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
-    <numFmt numFmtId="189" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;"/>
-    <numFmt numFmtId="190" formatCode="[DBNum1][$-404]General"/>
-    <numFmt numFmtId="191" formatCode="[DBNum2][$-404]General"/>
-    <numFmt numFmtId="192" formatCode="[$₩-412]#,##0.00"/>
-    <numFmt numFmtId="193" formatCode="[$₡-140A]#,##0.00"/>
-    <numFmt numFmtId="194" formatCode="[$₦-470]\ #,##0.00"/>
-    <numFmt numFmtId="195" formatCode="_-* #,##0.00\ [$₮-450]_-;\-* #,##0.00\ [$₮-450]_-;_-* &quot;-&quot;??\ [$₮-450]_-;_-@_-"/>
-    <numFmt numFmtId="196" formatCode="_([$₱-464]* #,##0.00_);_([$₱-464]* \(#,##0.00\);_([$₱-464]* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="197" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
-    <numFmt numFmtId="198" formatCode="yyyy\-mm\-dd;@"/>
-    <numFmt numFmtId="199" formatCode="m/d/yy;@"/>
-    <numFmt numFmtId="200" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="201" formatCode="[$-409]mmmm\-yy;@"/>
-    <numFmt numFmtId="202" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="203" formatCode="m/d/yy\ h:mm;@"/>
-    <numFmt numFmtId="204" formatCode="[$-409]mmmmm;@"/>
-    <numFmt numFmtId="205" formatCode="[$-409]mmmmm\-yy;@"/>
-    <numFmt numFmtId="206" formatCode="[$-409]d\-mmm\-yyyy;@"/>
-    <numFmt numFmtId="207" formatCode="*0###"/>
-    <numFmt numFmtId="208" formatCode="###* ###"/>
-    <numFmt numFmtId="209" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
-    <numFmt numFmtId="210" formatCode="yyyy/m/d\ h:mm;@"/>
-    <numFmt numFmtId="214" formatCode="[$$-404]#,##0.00;[Red]\-[$$-404]#,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="166" formatCode="m/d;@"/>
+    <numFmt numFmtId="167" formatCode="h:mm;@"/>
+    <numFmt numFmtId="168" formatCode="[$-409]d\-mmm;@"/>
+    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="170" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="171" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="172" formatCode="&quot;NT$&quot;#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="_-[$¥-411]* #,##0.00_-;\-[$¥-411]* #,##0.00_-;_-[$¥-411]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="174" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="175" formatCode="_(&quot;US$&quot;* #,##0.00_);_(&quot;US$&quot;* \(#,##0.00\);_(&quot;US$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
+    <numFmt numFmtId="178" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="179" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="180" formatCode="h:mm:ss;@"/>
+    <numFmt numFmtId="181" formatCode="0.0%"/>
+    <numFmt numFmtId="182" formatCode="0.000000%"/>
+    <numFmt numFmtId="183" formatCode="#\ ???/???"/>
+    <numFmt numFmtId="184" formatCode="0.E+00"/>
+    <numFmt numFmtId="185" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="186" formatCode="00000\-0000"/>
+    <numFmt numFmtId="187" formatCode="[&lt;=9999999]###\-####;\(0#\)\ ###\-####"/>
+    <numFmt numFmtId="188" formatCode="上午/下午h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;"/>
+    <numFmt numFmtId="189" formatCode="[DBNum1][$-404]General"/>
+    <numFmt numFmtId="190" formatCode="[DBNum2][$-404]General"/>
+    <numFmt numFmtId="191" formatCode="[$₩-412]#,##0.00"/>
+    <numFmt numFmtId="192" formatCode="[$₡-140A]#,##0.00"/>
+    <numFmt numFmtId="193" formatCode="[$₦-470]\ #,##0.00"/>
+    <numFmt numFmtId="194" formatCode="_-* #,##0.00\ [$₮-450]_-;\-* #,##0.00\ [$₮-450]_-;_-* &quot;-&quot;??\ [$₮-450]_-;_-@_-"/>
+    <numFmt numFmtId="195" formatCode="_([$₱-464]* #,##0.00_);_([$₱-464]* \(#,##0.00\);_([$₱-464]* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="196" formatCode="h&quot;時&quot;mm&quot;分&quot;ss&quot;秒&quot;;@"/>
+    <numFmt numFmtId="197" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="198" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="199" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="200" formatCode="[$-409]mmmm\-yy;@"/>
+    <numFmt numFmtId="201" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="202" formatCode="m/d/yy\ h:mm;@"/>
+    <numFmt numFmtId="203" formatCode="[$-409]mmmmm;@"/>
+    <numFmt numFmtId="204" formatCode="[$-409]mmmmm\-yy;@"/>
+    <numFmt numFmtId="205" formatCode="[$-409]d\-mmm\-yyyy;@"/>
+    <numFmt numFmtId="206" formatCode="*0###"/>
+    <numFmt numFmtId="207" formatCode="###* ###"/>
+    <numFmt numFmtId="208" formatCode="[$-409]yyyy/m/d\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="209" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="210" formatCode="[$$-404]#,##0.00;[Red]\-[$$-404]#,##0.00"/>
   </numFmts>
   <fonts count="51" x14ac:knownFonts="1">
     <font>
@@ -1393,7 +1393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
@@ -1520,11 +1520,11 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="8" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -1602,31 +1602,31 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="8" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="8" fontId="21" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="8" fontId="21" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
+    <xf numFmtId="8" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="8" fontId="26" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="8" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
@@ -1637,7 +1637,7 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="8" fontId="26" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1645,7 +1645,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="8" fontId="27" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1661,7 +1661,7 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1689,7 +1689,7 @@
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="168" fontId="32" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="32" fillId="4" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="4" borderId="13" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1755,53 +1755,53 @@
     <xf numFmtId="14" fontId="38" fillId="5" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="38" fillId="5" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="169" fontId="32" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="32" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="32" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="32" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="32" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="32" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="32" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="170" fontId="32" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="32" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="32" fillId="6" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="32" fillId="7" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="32" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="32" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="189" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="188" fontId="42" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="171" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="40" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="189" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="190" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="172" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="40" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="190" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="191" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="173" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="174" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="175" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="177" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="178" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="179" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="180" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="181" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="182" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="13" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="183" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="13" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="184" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="185" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="186" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="187" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="188" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="191" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="192" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="193" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="194" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="195" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="196" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="197" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2007,10 +2007,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="150" wrapText="1"/>
     </xf>
+    <xf numFmtId="197" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="198" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="199" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="200" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="201" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="202" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -2019,10 +2020,10 @@
     <xf numFmtId="205" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="206" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="207" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="208" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="190" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="189" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="208" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="209" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="210" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="37" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2048,7 +2049,6 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="214" fontId="42" fillId="10" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -13074,7 +13074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -13140,7 +13140,7 @@
       <c r="A5" s="113">
         <v>1234.56</v>
       </c>
-      <c r="B5" s="229">
+      <c r="B5" s="223">
         <v>-1234.56</v>
       </c>
       <c r="C5" s="132">
@@ -17978,14 +17978,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="224" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="224"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="224"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="89"/>
@@ -20501,16 +20501,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="7.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="6.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="2.83203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="31.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="1" customWidth="1"/>
@@ -20538,8 +20538,8 @@
         <v>32</v>
       </c>
       <c r="K1" s="2"/>
-      <c r="L1" s="227"/>
-      <c r="M1" s="227"/>
+      <c r="L1" s="228"/>
+      <c r="M1" s="228"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
@@ -20558,11 +20558,11 @@
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15"/>
-      <c r="B3" s="225" t="s">
+      <c r="B3" s="226" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="225"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="226"/>
+      <c r="D3" s="226"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
@@ -20572,16 +20572,16 @@
         <v>34</v>
       </c>
       <c r="K3" s="9"/>
-      <c r="L3" s="228"/>
-      <c r="M3" s="228"/>
+      <c r="L3" s="229"/>
+      <c r="M3" s="229"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15"/>
-      <c r="B4" s="225" t="s">
+      <c r="B4" s="226" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="225"/>
-      <c r="D4" s="225"/>
+      <c r="C4" s="226"/>
+      <c r="D4" s="226"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
@@ -20591,16 +20591,16 @@
         <v>0</v>
       </c>
       <c r="K4" s="9"/>
-      <c r="L4" s="228"/>
-      <c r="M4" s="228"/>
+      <c r="L4" s="229"/>
+      <c r="M4" s="229"/>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
-      <c r="B5" s="226" t="s">
+      <c r="B5" s="227" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="226"/>
-      <c r="D5" s="226"/>
+      <c r="C5" s="227"/>
+      <c r="D5" s="227"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
@@ -20610,8 +20610,8 @@
         <v>1</v>
       </c>
       <c r="K5" s="9"/>
-      <c r="L5" s="228"/>
-      <c r="M5" s="228"/>
+      <c r="L5" s="229"/>
+      <c r="M5" s="229"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="11"/>
@@ -20645,10 +20645,10 @@
     </row>
     <row r="8" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
-      <c r="B8" s="224" t="s">
+      <c r="B8" s="225" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="224"/>
+      <c r="C8" s="225"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
       <c r="F8" s="18" t="s">

</xml_diff>